<commit_message>
version con revision de estilo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -356,7 +356,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1854,7 +1854,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1864,17 +1864,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -1941,7 +1941,7 @@
       <selection activeCell="A2" sqref="A2:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
@@ -1953,7 +1953,7 @@
     <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1">
       <c r="A2" s="29" t="s">
         <v>37</v>
       </c>
@@ -1999,7 +1999,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="29" t="s">
         <v>37</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="29" t="s">
         <v>37</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="29" t="s">
         <v>37</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="29" t="s">
         <v>37</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="29" t="s">
         <v>37</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="29" t="s">
         <v>37</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="29" t="s">
         <v>37</v>
       </c>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="29" t="s">
         <v>48</v>
       </c>
@@ -2161,7 +2161,7 @@
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="29" t="s">
         <v>54</v>
       </c>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="29" t="s">
         <v>55</v>
       </c>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="29" t="s">
         <v>64</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="29" t="s">
         <v>65</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="29" t="s">
         <v>66</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="29" t="s">
         <v>67</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="29" t="s">
         <v>68</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="29" t="s">
         <v>69</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="29" t="s">
         <v>70</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="29" t="s">
         <v>71</v>
       </c>
@@ -2382,13 +2382,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="66.140625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>72</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1">
       <c r="A3" s="13" t="s">
         <v>73</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
@@ -2464,18 +2464,18 @@
   </sheetPr>
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="92.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -2494,10 +2494,10 @@
         <v>38</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -2505,10 +2505,10 @@
         <v>40</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -2516,10 +2516,10 @@
         <v>42</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -2538,10 +2538,10 @@
         <v>43</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -2549,10 +2549,10 @@
         <v>44</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -2560,10 +2560,10 @@
         <v>45</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -2571,10 +2571,10 @@
         <v>46</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -2582,10 +2582,10 @@
         <v>47</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -2593,10 +2593,10 @@
         <v>50</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -2604,10 +2604,10 @@
         <v>52</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -2615,10 +2615,10 @@
         <v>53</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -2626,10 +2626,10 @@
         <v>73</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="14">
         <v>14</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -2648,10 +2648,10 @@
         <v>57</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="14">
         <v>16</v>
       </c>
@@ -2659,10 +2659,10 @@
         <v>58</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -2681,10 +2681,10 @@
         <v>60</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -2692,10 +2692,10 @@
         <v>61</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -2703,10 +2703,10 @@
         <v>62</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="14">
         <v>23</v>
       </c>
@@ -2739,77 +2739,77 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="73"/>
       <c r="B25" s="73"/>
       <c r="C25" s="71"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="62"/>
       <c r="B26" s="62"/>
       <c r="C26" s="71"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="62"/>
       <c r="B27" s="62"/>
       <c r="C27" s="71"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="62"/>
       <c r="B28" s="62"/>
       <c r="C28" s="71"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="62"/>
       <c r="B29" s="62"/>
       <c r="C29" s="71"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="62"/>
       <c r="B30" s="62"/>
       <c r="C30" s="71"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="62"/>
       <c r="B31" s="62"/>
       <c r="C31" s="71"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="62"/>
       <c r="B32" s="62"/>
       <c r="C32" s="71"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="62"/>
       <c r="B33" s="62"/>
       <c r="C33" s="71"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="62"/>
       <c r="B34" s="62"/>
       <c r="C34" s="71"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="62"/>
       <c r="B35" s="62"/>
       <c r="C35" s="71"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="62"/>
       <c r="B36" s="62"/>
       <c r="C36" s="71"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="71"/>
       <c r="B37" s="71"/>
       <c r="C37" s="72"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="71"/>
       <c r="B38" s="71"/>
       <c r="C38" s="72"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="71"/>
       <c r="B39" s="71"/>
       <c r="C39" s="72"/>
@@ -2837,7 +2837,7 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="49" customWidth="1"/>
     <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
@@ -2848,7 +2848,7 @@
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="48" t="s">
         <v>6</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="47" t="s">
         <v>33</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="47" t="s">
         <v>33</v>
       </c>
@@ -2911,7 +2911,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="47" t="s">
         <v>33</v>
       </c>
@@ -2928,7 +2928,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="35" customFormat="1" ht="15.75">
       <c r="A5" s="47" t="s">
         <v>33</v>
       </c>
@@ -2947,7 +2947,7 @@
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
     </row>
-    <row r="6" spans="1:9" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="35" customFormat="1" ht="15.75">
       <c r="A6" s="47" t="s">
         <v>33</v>
       </c>
@@ -2964,7 +2964,7 @@
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="47" t="s">
         <v>33</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75">
       <c r="A8" s="47" t="s">
         <v>33</v>
       </c>
@@ -3004,7 +3004,7 @@
       <c r="H8" s="38"/>
       <c r="I8" s="38"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="47" t="s">
         <v>33</v>
       </c>
@@ -3023,7 +3023,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="47" t="s">
         <v>33</v>
       </c>
@@ -3040,7 +3040,7 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="47" t="s">
         <v>33</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75">
       <c r="A12" s="47" t="s">
         <v>33</v>
       </c>
@@ -3080,7 +3080,7 @@
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75">
       <c r="A13" s="47" t="s">
         <v>33</v>
       </c>
@@ -3097,7 +3097,7 @@
       <c r="H13" s="38"/>
       <c r="I13" s="38"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75">
       <c r="A14" s="47" t="s">
         <v>33</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="H14" s="38"/>
       <c r="I14" s="38"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75">
       <c r="A15" s="47" t="s">
         <v>33</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75">
       <c r="A16" s="47" t="s">
         <v>33</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="67" t="s">
         <v>33</v>
       </c>
@@ -3175,7 +3175,7 @@
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="68" t="s">
         <v>33</v>
       </c>
@@ -3192,7 +3192,7 @@
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.75">
       <c r="A19" s="50" t="s">
         <v>33</v>
       </c>
@@ -3209,7 +3209,7 @@
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="50" t="s">
         <v>33</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="50" t="s">
         <v>33</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="50" t="s">
         <v>33</v>
       </c>
@@ -3268,7 +3268,7 @@
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75">
       <c r="A23" s="50" t="s">
         <v>33</v>
       </c>
@@ -3285,7 +3285,7 @@
       <c r="H23" s="52"/>
       <c r="I23" s="52"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75">
       <c r="A24" s="50" t="s">
         <v>33</v>
       </c>
@@ -3302,7 +3302,7 @@
       <c r="H24" s="52"/>
       <c r="I24" s="52"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75">
       <c r="A25" s="50" t="s">
         <v>33</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="H25" s="52"/>
       <c r="I25" s="52"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.75">
       <c r="A26" s="50" t="s">
         <v>33</v>
       </c>
@@ -3338,7 +3338,7 @@
       <c r="H26" s="52"/>
       <c r="I26" s="52"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.75">
       <c r="A27" s="50" t="s">
         <v>33</v>
       </c>
@@ -3355,7 +3355,7 @@
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="50" t="s">
         <v>33</v>
       </c>
@@ -3370,7 +3370,7 @@
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="50" t="s">
         <v>33</v>
       </c>
@@ -3385,7 +3385,7 @@
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15.75">
       <c r="A30" s="50" t="s">
         <v>33</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15.75">
       <c r="A31" s="50" t="s">
         <v>33</v>
       </c>
@@ -3421,7 +3421,7 @@
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15.75">
       <c r="A32" s="50" t="s">
         <v>33</v>
       </c>
@@ -3438,7 +3438,7 @@
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15.75">
       <c r="A33" s="50" t="s">
         <v>33</v>
       </c>
@@ -3455,7 +3455,7 @@
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15.75">
       <c r="A34" s="50" t="s">
         <v>33</v>
       </c>
@@ -3474,7 +3474,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15.75">
       <c r="A35" s="50" t="s">
         <v>33</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15.75">
       <c r="A36" s="50" t="s">
         <v>33</v>
       </c>
@@ -3512,7 +3512,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="15.75">
       <c r="A37" s="50" t="s">
         <v>33</v>
       </c>
@@ -3529,7 +3529,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="15.75">
       <c r="A38" s="50" t="s">
         <v>33</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="15.75">
       <c r="A39" s="50" t="s">
         <v>33</v>
       </c>
@@ -3569,7 +3569,7 @@
       <c r="H39" s="57"/>
       <c r="I39" s="57"/>
     </row>
-    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="15.75">
       <c r="A40" s="50" t="s">
         <v>33</v>
       </c>
@@ -3586,7 +3586,7 @@
       <c r="H40" s="57"/>
       <c r="I40" s="57"/>
     </row>
-    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="15.75">
       <c r="A41" s="50" t="s">
         <v>33</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="15.75">
       <c r="A42" s="50" t="s">
         <v>33</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="15.75">
       <c r="A43" s="50" t="s">
         <v>33</v>
       </c>
@@ -3645,7 +3645,7 @@
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
     </row>
-    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="15.75">
       <c r="A44" s="50" t="s">
         <v>33</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="15.75">
       <c r="A45" s="50" t="s">
         <v>33</v>
       </c>
@@ -3683,7 +3683,7 @@
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
     </row>
-    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="15.75">
       <c r="A46" s="50" t="s">
         <v>33</v>
       </c>
@@ -3702,7 +3702,7 @@
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>
     </row>
-    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="15.75">
       <c r="A47" s="50" t="s">
         <v>33</v>
       </c>
@@ -3719,7 +3719,7 @@
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
     </row>
-    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="15.75">
       <c r="A48" s="50" t="s">
         <v>33</v>
       </c>
@@ -3736,7 +3736,7 @@
       <c r="H48" s="15"/>
       <c r="I48" s="15"/>
     </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="15.75">
       <c r="A49" s="50" t="s">
         <v>33</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="15.75">
       <c r="A50" s="50" t="s">
         <v>33</v>
       </c>
@@ -3776,7 +3776,7 @@
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15.75">
       <c r="A51" s="50" t="s">
         <v>33</v>
       </c>
@@ -3793,7 +3793,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="50" t="s">
         <v>33</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="50" t="s">
         <v>33</v>
       </c>
@@ -3827,7 +3827,7 @@
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" s="50" t="s">
         <v>33</v>
       </c>
@@ -3842,7 +3842,7 @@
       <c r="H54" s="14"/>
       <c r="I54" s="14"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="50" t="s">
         <v>33</v>
       </c>
@@ -3857,7 +3857,7 @@
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" s="50" t="s">
         <v>33</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" s="50" t="s">
         <v>33</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" s="50" t="s">
         <v>33</v>
       </c>
@@ -3912,7 +3912,7 @@
       <c r="H58" s="14"/>
       <c r="I58" s="14"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" s="50" t="s">
         <v>33</v>
       </c>
@@ -3927,7 +3927,7 @@
       <c r="H59" s="23"/>
       <c r="I59" s="23"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" s="50" t="s">
         <v>33</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="H60" s="14"/>
       <c r="I60" s="14"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" s="50" t="s">
         <v>33</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="A62" s="50" t="s">
         <v>33</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9">
       <c r="A63" s="50" t="s">
         <v>33</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64" s="50" t="s">
         <v>33</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9">
       <c r="A65" s="50" t="s">
         <v>33</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9">
       <c r="A66" s="50" t="s">
         <v>33</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9">
       <c r="A67" s="50" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Revert "version con revision de estilo"
This reverts commit e9606bce6e283e8f5ef344f1736e602b4699dbfe.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -356,7 +356,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1854,7 +1854,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1864,17 +1864,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -1941,7 +1941,7 @@
       <selection activeCell="A2" sqref="A2:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
@@ -1953,7 +1953,7 @@
     <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>37</v>
       </c>
@@ -1999,7 +1999,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>37</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>37</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>37</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>37</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>37</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>37</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>37</v>
       </c>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>48</v>
       </c>
@@ -2161,7 +2161,7 @@
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>54</v>
       </c>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>55</v>
       </c>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>64</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>65</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>66</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>67</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>68</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>69</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>70</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>71</v>
       </c>
@@ -2382,13 +2382,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.140625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>72</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>73</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
@@ -2464,18 +2464,18 @@
   </sheetPr>
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C14" sqref="B14:C14"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="92.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -2494,10 +2494,10 @@
         <v>38</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -2505,10 +2505,10 @@
         <v>40</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -2516,10 +2516,10 @@
         <v>42</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -2538,10 +2538,10 @@
         <v>43</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -2549,10 +2549,10 @@
         <v>44</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -2560,10 +2560,10 @@
         <v>45</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -2571,10 +2571,10 @@
         <v>46</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -2582,10 +2582,10 @@
         <v>47</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -2593,10 +2593,10 @@
         <v>50</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -2604,10 +2604,10 @@
         <v>52</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -2615,10 +2615,10 @@
         <v>53</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -2626,10 +2626,10 @@
         <v>73</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>14</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -2648,10 +2648,10 @@
         <v>57</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>16</v>
       </c>
@@ -2659,10 +2659,10 @@
         <v>58</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -2681,10 +2681,10 @@
         <v>60</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -2692,10 +2692,10 @@
         <v>61</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -2703,10 +2703,10 @@
         <v>62</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>23</v>
       </c>
@@ -2739,77 +2739,77 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="73"/>
       <c r="B25" s="73"/>
       <c r="C25" s="71"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="62"/>
       <c r="B26" s="62"/>
       <c r="C26" s="71"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="62"/>
       <c r="B27" s="62"/>
       <c r="C27" s="71"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="62"/>
       <c r="B28" s="62"/>
       <c r="C28" s="71"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="62"/>
       <c r="B29" s="62"/>
       <c r="C29" s="71"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="62"/>
       <c r="B30" s="62"/>
       <c r="C30" s="71"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="62"/>
       <c r="B31" s="62"/>
       <c r="C31" s="71"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="62"/>
       <c r="B32" s="62"/>
       <c r="C32" s="71"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="62"/>
       <c r="B33" s="62"/>
       <c r="C33" s="71"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="62"/>
       <c r="B34" s="62"/>
       <c r="C34" s="71"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="62"/>
       <c r="B35" s="62"/>
       <c r="C35" s="71"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="62"/>
       <c r="B36" s="62"/>
       <c r="C36" s="71"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="71"/>
       <c r="B37" s="71"/>
       <c r="C37" s="72"/>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="71"/>
       <c r="B38" s="71"/>
       <c r="C38" s="72"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="71"/>
       <c r="B39" s="71"/>
       <c r="C39" s="72"/>
@@ -2837,7 +2837,7 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="49" customWidth="1"/>
     <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
@@ -2848,7 +2848,7 @@
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>6</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>33</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>33</v>
       </c>
@@ -2911,7 +2911,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>33</v>
       </c>
@@ -2928,7 +2928,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" s="35" customFormat="1" ht="15.75">
+    <row r="5" spans="1:9" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>33</v>
       </c>
@@ -2947,7 +2947,7 @@
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
     </row>
-    <row r="6" spans="1:9" s="35" customFormat="1" ht="15.75">
+    <row r="6" spans="1:9" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>33</v>
       </c>
@@ -2964,7 +2964,7 @@
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>33</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>33</v>
       </c>
@@ -3004,7 +3004,7 @@
       <c r="H8" s="38"/>
       <c r="I8" s="38"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>33</v>
       </c>
@@ -3023,7 +3023,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>33</v>
       </c>
@@ -3040,7 +3040,7 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>33</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
         <v>33</v>
       </c>
@@ -3080,7 +3080,7 @@
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
         <v>33</v>
       </c>
@@ -3097,7 +3097,7 @@
       <c r="H13" s="38"/>
       <c r="I13" s="38"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
         <v>33</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="H14" s="38"/>
       <c r="I14" s="38"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
         <v>33</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
         <v>33</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75">
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="67" t="s">
         <v>33</v>
       </c>
@@ -3175,7 +3175,7 @@
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="68" t="s">
         <v>33</v>
       </c>
@@ -3192,7 +3192,7 @@
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
         <v>33</v>
       </c>
@@ -3209,7 +3209,7 @@
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
         <v>33</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75">
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
         <v>33</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="50" t="s">
         <v>33</v>
       </c>
@@ -3268,7 +3268,7 @@
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="50" t="s">
         <v>33</v>
       </c>
@@ -3285,7 +3285,7 @@
       <c r="H23" s="52"/>
       <c r="I23" s="52"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="50" t="s">
         <v>33</v>
       </c>
@@ -3302,7 +3302,7 @@
       <c r="H24" s="52"/>
       <c r="I24" s="52"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="50" t="s">
         <v>33</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="H25" s="52"/>
       <c r="I25" s="52"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75">
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="50" t="s">
         <v>33</v>
       </c>
@@ -3338,7 +3338,7 @@
       <c r="H26" s="52"/>
       <c r="I26" s="52"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75">
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="50" t="s">
         <v>33</v>
       </c>
@@ -3355,7 +3355,7 @@
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="50" t="s">
         <v>33</v>
       </c>
@@ -3370,7 +3370,7 @@
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="50" t="s">
         <v>33</v>
       </c>
@@ -3385,7 +3385,7 @@
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75">
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="50" t="s">
         <v>33</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75">
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="50" t="s">
         <v>33</v>
       </c>
@@ -3421,7 +3421,7 @@
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" ht="15.75">
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="50" t="s">
         <v>33</v>
       </c>
@@ -3438,7 +3438,7 @@
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75">
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="50" t="s">
         <v>33</v>
       </c>
@@ -3455,7 +3455,7 @@
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75">
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="50" t="s">
         <v>33</v>
       </c>
@@ -3474,7 +3474,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" ht="15.75">
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="50" t="s">
         <v>33</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75">
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="50" t="s">
         <v>33</v>
       </c>
@@ -3512,7 +3512,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" ht="15.75">
+    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="50" t="s">
         <v>33</v>
       </c>
@@ -3529,7 +3529,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" ht="15.75">
+    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="50" t="s">
         <v>33</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75">
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="50" t="s">
         <v>33</v>
       </c>
@@ -3569,7 +3569,7 @@
       <c r="H39" s="57"/>
       <c r="I39" s="57"/>
     </row>
-    <row r="40" spans="1:9" ht="15.75">
+    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="50" t="s">
         <v>33</v>
       </c>
@@ -3586,7 +3586,7 @@
       <c r="H40" s="57"/>
       <c r="I40" s="57"/>
     </row>
-    <row r="41" spans="1:9" ht="15.75">
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="50" t="s">
         <v>33</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75">
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="50" t="s">
         <v>33</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75">
+    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="50" t="s">
         <v>33</v>
       </c>
@@ -3645,7 +3645,7 @@
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
     </row>
-    <row r="44" spans="1:9" ht="15.75">
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="50" t="s">
         <v>33</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75">
+    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="50" t="s">
         <v>33</v>
       </c>
@@ -3683,7 +3683,7 @@
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
     </row>
-    <row r="46" spans="1:9" ht="15.75">
+    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="50" t="s">
         <v>33</v>
       </c>
@@ -3702,7 +3702,7 @@
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>
     </row>
-    <row r="47" spans="1:9" ht="15.75">
+    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="50" t="s">
         <v>33</v>
       </c>
@@ -3719,7 +3719,7 @@
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
     </row>
-    <row r="48" spans="1:9" ht="15.75">
+    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="50" t="s">
         <v>33</v>
       </c>
@@ -3736,7 +3736,7 @@
       <c r="H48" s="15"/>
       <c r="I48" s="15"/>
     </row>
-    <row r="49" spans="1:9" ht="15.75">
+    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="50" t="s">
         <v>33</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75">
+    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="50" t="s">
         <v>33</v>
       </c>
@@ -3776,7 +3776,7 @@
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75">
+    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="50" t="s">
         <v>33</v>
       </c>
@@ -3793,7 +3793,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="50" t="s">
         <v>33</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="50" t="s">
         <v>33</v>
       </c>
@@ -3827,7 +3827,7 @@
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="50" t="s">
         <v>33</v>
       </c>
@@ -3842,7 +3842,7 @@
       <c r="H54" s="14"/>
       <c r="I54" s="14"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="50" t="s">
         <v>33</v>
       </c>
@@ -3857,7 +3857,7 @@
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="50" t="s">
         <v>33</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="50" t="s">
         <v>33</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="50" t="s">
         <v>33</v>
       </c>
@@ -3912,7 +3912,7 @@
       <c r="H58" s="14"/>
       <c r="I58" s="14"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="50" t="s">
         <v>33</v>
       </c>
@@ -3927,7 +3927,7 @@
       <c r="H59" s="23"/>
       <c r="I59" s="23"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="50" t="s">
         <v>33</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="H60" s="14"/>
       <c r="I60" s="14"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="50" t="s">
         <v>33</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="50" t="s">
         <v>33</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="50" t="s">
         <v>33</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="50" t="s">
         <v>33</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="50" t="s">
         <v>33</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="50" t="s">
         <v>33</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="50" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Esqueleto y Guion 1 Grado 8_Con revision
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="106">
   <si>
     <t>FICHA</t>
   </si>
@@ -119,12 +119,6 @@
   </si>
   <si>
     <t>Recuerda</t>
-  </si>
-  <si>
-    <t>Educación secundaria obligatoria</t>
-  </si>
-  <si>
-    <t>Ciencias sociales, geografía e historia</t>
   </si>
   <si>
     <t>El pensamiento liberal y las revoluciones</t>
@@ -283,9 +277,6 @@
     <t>La sociedad del Antiguo Régimen</t>
   </si>
   <si>
-    <t>Imagen</t>
-  </si>
-  <si>
     <t>La economía del siglo XVIII</t>
   </si>
   <si>
@@ -350,13 +341,28 @@
   </si>
   <si>
     <t xml:space="preserve">Cronología: el fin del Antiguo Régimen </t>
+  </si>
+  <si>
+    <t>Educación Básica Secundaria</t>
+  </si>
+  <si>
+    <t>Ciencias Sociales</t>
+  </si>
+  <si>
+    <t>Consolidación</t>
+  </si>
+  <si>
+    <t>Consolidacion</t>
+  </si>
+  <si>
+    <t>Las Revoluciones inglesas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,6 +424,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -427,13 +434,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -481,7 +481,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -544,19 +544,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,6 +557,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1039,7 +1057,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1070,118 +1088,152 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1854,7 +1906,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1864,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,39 +1930,39 @@
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>33</v>
+      <c r="B1" s="42" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
+      <c r="B2" s="43" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>35</v>
+      <c r="B3" s="44" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>31</v>
+      <c r="B4" s="43" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="43">
         <v>8</v>
       </c>
     </row>
@@ -1918,8 +1970,8 @@
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
+      <c r="B6" s="43" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1974,22 +2026,22 @@
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="29">
+      <c r="F2" s="19">
         <v>1</v>
       </c>
       <c r="G2"/>
@@ -2000,366 +2052,366 @@
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="F3" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C4" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="29" t="s">
+      <c r="E5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="D6" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="F6" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="29" t="s">
+      <c r="C7" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="D7" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="F7" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="29" t="s">
+      <c r="C8" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="D8" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="F8" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="29" t="s">
+      <c r="C9" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="D9" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="F9" s="19">
+        <v>9</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="29" t="s">
+      <c r="C10" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="19">
+        <v>10</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="29">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="D11" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="F11" s="19">
+        <v>11</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="29" t="s">
+      <c r="C12" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="29">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="D12" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="F12" s="19">
+        <v>12</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="29" t="s">
+      <c r="C13" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="29">
-        <v>9</v>
-      </c>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="29" t="s">
+      <c r="D13" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="29">
-        <v>10</v>
-      </c>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="29" t="s">
+      <c r="C14" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="29" t="s">
+      <c r="C15" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="29">
-        <v>11</v>
-      </c>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="29" t="s">
+      <c r="D15" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="29" t="s">
+      <c r="C16" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="29">
-        <v>12</v>
-      </c>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="29" t="s">
+      <c r="D16" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="29" t="s">
+      <c r="C17" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="29">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="29" t="s">
+      <c r="D17" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="29" t="s">
+      <c r="C18" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="29">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="29" t="s">
+      <c r="D18" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="19">
         <v>19</v>
       </c>
-      <c r="C15" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="29" t="s">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="29">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="29" t="s">
+      <c r="D19" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="29" t="s">
+      <c r="C20" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="29">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="29">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="29" t="s">
+      <c r="D20" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="29">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="29">
+      <c r="E20" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="19">
         <v>21</v>
       </c>
     </row>
@@ -2401,7 +2453,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>21</v>
@@ -2412,7 +2464,7 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>21</v>
@@ -2491,7 +2543,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>21</v>
@@ -2502,7 +2554,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>21</v>
@@ -2513,7 +2565,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>21</v>
@@ -2524,7 +2576,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>21</v>
@@ -2535,7 +2587,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>21</v>
@@ -2546,7 +2598,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>21</v>
@@ -2557,7 +2609,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>21</v>
@@ -2568,7 +2620,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>21</v>
@@ -2579,7 +2631,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>21</v>
@@ -2590,7 +2642,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>21</v>
@@ -2601,7 +2653,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>21</v>
@@ -2612,7 +2664,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>21</v>
@@ -2623,7 +2675,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>20</v>
@@ -2634,7 +2686,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>20</v>
@@ -2645,7 +2697,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>21</v>
@@ -2656,7 +2708,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>21</v>
@@ -2667,7 +2719,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>20</v>
@@ -2678,7 +2730,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>21</v>
@@ -2689,7 +2741,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>21</v>
@@ -2700,7 +2752,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>21</v>
@@ -2711,7 +2763,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>21</v>
@@ -2740,79 +2792,79 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="73"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="71"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="39"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="71"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="39"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="62"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="71"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="39"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="62"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="71"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="39"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="71"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="39"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
-      <c r="B30" s="62"/>
-      <c r="C30" s="71"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="39"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="71"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="39"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="71"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="39"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="71"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="39"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="62"/>
-      <c r="B34" s="62"/>
-      <c r="C34" s="71"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="39"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="62"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="71"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="39"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="62"/>
-      <c r="B36" s="62"/>
-      <c r="C36" s="71"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="39"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="71"/>
-      <c r="B37" s="71"/>
-      <c r="C37" s="72"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="40"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="71"/>
-      <c r="B38" s="71"/>
-      <c r="C38" s="72"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="40"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="71"/>
-      <c r="B39" s="71"/>
-      <c r="C39" s="72"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="40"/>
     </row>
   </sheetData>
   <sortState ref="A2:C38">
@@ -2831,15 +2883,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="49" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="29" customWidth="1"/>
     <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
@@ -2849,7 +2901,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -2878,1214 +2930,1237 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="32" t="s">
+      <c r="A2" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="32" t="s">
+      <c r="A3" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="33" t="s">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+    </row>
+    <row r="7" spans="1:9" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="65" t="s">
+      <c r="E10" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E13" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-    </row>
-    <row r="6" spans="1:9" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37" t="s">
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="39" t="s">
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="37" t="s">
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="63" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37" t="s">
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="I17" s="66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="17" t="s">
+      <c r="D18" s="82"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="36" t="s">
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="81" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="81" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" s="81" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="36" t="s">
+      <c r="D22" s="83"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="69"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="81" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="83"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="81"/>
+      <c r="H23" s="81" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="81" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="85"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="85"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="66"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="66"/>
+      <c r="D26" s="70" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="66"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="58"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="I31" s="58" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="84"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="59"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="59"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="59"/>
+      <c r="D35" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="66"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="59"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="I36" s="66" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="59"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="66"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="59"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="66"/>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="59"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="I11" s="13" t="s">
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="I39" s="66" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="61" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="39" t="s">
+    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="59"/>
+      <c r="D40" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="39" t="s">
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="59"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="59"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I42" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="59"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="I43" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="38" t="s">
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I45" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16" s="46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="69" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="16" t="s">
+    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="69" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="69" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="69" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="69" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="69" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="53"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="52"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="I30" s="19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="I35" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="I38" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="57" t="s">
-        <v>24</v>
-      </c>
-      <c r="F39" s="57"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="57"/>
-      <c r="I39" s="57"/>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B40" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" s="57"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="57"/>
-      <c r="I40" s="57"/>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" s="57"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="I41" s="57" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="F42" s="57"/>
-      <c r="G42" s="57"/>
-      <c r="H42" s="58" t="s">
-        <v>90</v>
-      </c>
-      <c r="I42" s="57" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="I44" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>24</v>
-      </c>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" s="70" t="s">
+      <c r="A47" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="63"/>
+      <c r="G47" s="63"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="63"/>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="15"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="63"/>
+      <c r="G48" s="63"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="63"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49" s="63"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="63"/>
+      <c r="I49" s="63"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" s="63"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="I50" s="63" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B49" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="I49" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B50" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E50" s="15" t="s">
+      <c r="E51" s="15" t="s">
         <v>24</v>
-      </c>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-    </row>
-    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B51" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15" t="s">
-        <v>27</v>
       </c>
       <c r="F51" s="15"/>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
+    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="15"/>
       <c r="D52" s="15"/>
       <c r="E52" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F52" s="15"/>
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
-      <c r="I52" s="15" t="s">
+      <c r="I52" s="15"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="E53" s="14" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14" t="s">
-        <v>25</v>
-      </c>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
       <c r="F54" s="14"/>
       <c r="G54" s="14"/>
       <c r="H54" s="14"/>
       <c r="I54" s="14"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
+      <c r="A55" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="D55" s="14"/>
-      <c r="E55" s="14" t="s">
-        <v>24</v>
-      </c>
+      <c r="E55" s="21"/>
       <c r="F55" s="14"/>
       <c r="G55" s="14"/>
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
+      <c r="A56" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="D56" s="14"/>
-      <c r="E56" s="14" t="s">
+      <c r="E56" s="21"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F56" s="22"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="I56" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
       <c r="D57" s="14"/>
-      <c r="E57" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F57" s="22"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="17"/>
       <c r="G57" s="14"/>
       <c r="H57" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I57" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="63" t="s">
+      <c r="A58" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="I58" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="78" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="89"/>
+      <c r="G59" s="47"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="47"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="78" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="90"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="90"/>
+      <c r="H60" s="90"/>
+      <c r="I60" s="90"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="78" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D61" s="47"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="78" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="47"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="47"/>
+      <c r="H62" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="I62" s="47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" s="78" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="47"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="47"/>
+      <c r="H63" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="I63" s="47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64" s="78" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="47"/>
+      <c r="H64" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="I64" s="47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="E58" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F58" s="22"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
-      <c r="E59" s="59" t="s">
-        <v>25</v>
-      </c>
-      <c r="F59" s="24"/>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23"/>
-      <c r="I59" s="23"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="I61" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="I62" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="I63" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F64" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G64" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H64" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="I64" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>101</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
-      <c r="E65" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F65" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G65" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
       <c r="H65" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I65" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B66" s="26" t="s">
+      <c r="A66" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I66" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C66" s="26" t="s">
+      <c r="C67" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D66" s="26"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="26"/>
-      <c r="G66" s="26"/>
-      <c r="H66" s="26"/>
-      <c r="I66" s="26" t="s">
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B67" s="26" t="s">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C68" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D67" s="26"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="26"/>
-      <c r="G67" s="26"/>
-      <c r="H67" s="26" t="s">
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I67" s="26" t="s">
+      <c r="I68" s="18" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
esqueleto Grado 8-Guion 1
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="106">
   <si>
     <t>FICHA</t>
   </si>
@@ -453,7 +453,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,12 +470,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -504,19 +498,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,25 +522,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1029,7 +1005,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1057,45 +1033,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1103,111 +1062,117 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1880,7 +1845,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1904,7 +1869,7 @@
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="29" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1912,7 +1877,7 @@
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="30" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1920,7 +1885,7 @@
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="31" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1928,7 +1893,7 @@
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="30" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1936,7 +1901,7 @@
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="30">
         <v>8</v>
       </c>
     </row>
@@ -1944,7 +1909,7 @@
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="30" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2000,22 +1965,22 @@
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="17">
         <v>1</v>
       </c>
       <c r="G2"/>
@@ -2026,366 +1991,366 @@
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="17">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="17">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <v>9</v>
       </c>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <v>10</v>
       </c>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <v>11</v>
       </c>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <v>12</v>
       </c>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="17">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="17">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="17">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="17">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="17">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="17">
         <v>21</v>
       </c>
     </row>
@@ -2643,7 +2608,7 @@
       <c r="C13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="60"/>
+      <c r="D13" s="34"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
@@ -2767,79 +2732,79 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="35"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="26"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="35"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="35"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="35"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="26"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="35"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="35"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="35"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="35"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="35"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="35"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="35"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="26"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="35"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="26"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="36"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="27"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="36"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="27"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="36"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="27"/>
     </row>
   </sheetData>
   <sortState ref="A2:C38">
@@ -2860,13 +2825,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D9"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="27" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="23" customWidth="1"/>
     <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
@@ -2877,16 +2842,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="39" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="36" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="8" t="s">
@@ -2906,118 +2871,120 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="59" t="s">
+      <c r="A2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="59" t="s">
+      <c r="A3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="59" t="s">
+      <c r="A4" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="59" t="s">
+      <c r="A5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="59" t="s">
+    <row r="6" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="91" t="s">
+      <c r="C6" s="41"/>
+      <c r="D6" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-    </row>
-    <row r="7" spans="1:9" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="59" t="s">
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="91" t="s">
+      <c r="C7" s="41"/>
+      <c r="D7" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="59" t="s">
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="91" t="s">
+      <c r="C8" s="43"/>
+      <c r="D8" s="40" t="s">
         <v>103</v>
       </c>
       <c r="E8" s="44" t="s">
@@ -3028,704 +2995,703 @@
       <c r="H8" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="41" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="59" t="s">
+    <row r="9" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="91" t="s">
+      <c r="C9" s="47"/>
+      <c r="D9" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="59" t="s">
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="73" t="s">
+      <c r="C10" s="47"/>
+      <c r="D10" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="E10" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="59" t="s">
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+    </row>
+    <row r="11" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="73" t="s">
+      <c r="C11" s="47"/>
+      <c r="D11" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="59" t="s">
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="73" t="s">
+      <c r="C12" s="47"/>
+      <c r="D12" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="51" t="s">
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="49" t="s">
+      <c r="I12" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="59" t="s">
+    <row r="13" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="74" t="s">
+      <c r="C13" s="47"/>
+      <c r="D13" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="59" t="s">
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="74" t="s">
+      <c r="C14" s="47"/>
+      <c r="D14" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E14" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="59" t="s">
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="74" t="s">
+      <c r="C15" s="47"/>
+      <c r="D15" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="59" t="s">
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="74" t="s">
+      <c r="C16" s="47"/>
+      <c r="D16" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="57" t="s">
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="56" t="s">
+      <c r="I16" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="59" t="s">
+    <row r="17" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="64" t="s">
+      <c r="C17" s="49"/>
+      <c r="D17" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="57" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="49" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="67" t="s">
+    <row r="18" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="65" t="s">
+      <c r="C18" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="66"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="67" t="s">
+      <c r="D18" s="63"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="62"/>
+    </row>
+    <row r="19" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="65" t="s">
+      <c r="C19" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="76"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="67" t="s">
+      <c r="D19" s="65"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+    </row>
+    <row r="20" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="65" t="s">
+      <c r="C20" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="76"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="67" t="s">
+      <c r="D20" s="65"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+    </row>
+    <row r="21" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="65" t="s">
+      <c r="C21" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="76"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65" t="s">
+      <c r="D21" s="65"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="I21" s="65" t="s">
+      <c r="I21" s="62" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="67" t="s">
+    <row r="22" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="61"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="67" t="s">
+      <c r="D22" s="67"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="I22" s="68"/>
+    </row>
+    <row r="23" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="77"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65" t="s">
+      <c r="D23" s="67"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="65" t="s">
+      <c r="I23" s="62" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="68" t="s">
+    <row r="24" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="58" t="s">
+      <c r="C24" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="78"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="68" t="s">
+      <c r="D24" s="37"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+    </row>
+    <row r="25" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="58" t="s">
+      <c r="C25" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="78"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="68" t="s">
+      <c r="D25" s="37"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+    </row>
+    <row r="26" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="88" t="s">
+      <c r="C26" s="32"/>
+      <c r="D26" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="68" t="s">
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+    </row>
+    <row r="27" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="88" t="s">
+      <c r="C27" s="32"/>
+      <c r="D27" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="68" t="s">
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+    </row>
+    <row r="28" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="58"/>
-      <c r="D28" s="89" t="s">
+      <c r="C28" s="32"/>
+      <c r="D28" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="52" t="s">
+      <c r="E28" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="68" t="s">
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+    </row>
+    <row r="29" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="58"/>
-      <c r="D29" s="89" t="s">
+      <c r="C29" s="32"/>
+      <c r="D29" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="52" t="s">
+      <c r="E29" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="68" t="s">
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+    </row>
+    <row r="30" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="58"/>
-      <c r="D30" s="89" t="s">
+      <c r="C30" s="32"/>
+      <c r="D30" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="52" t="s">
+      <c r="E30" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="68" t="s">
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+    </row>
+    <row r="31" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="58"/>
-      <c r="D31" s="62" t="s">
+      <c r="C31" s="32"/>
+      <c r="D31" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E31" s="72" t="s">
+      <c r="E31" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="63" t="s">
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="I31" s="52" t="s">
+      <c r="I31" s="32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="86" t="s">
+    <row r="32" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="53" t="s">
+      <c r="C32" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="79"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="86" t="s">
+      <c r="D32" s="72"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+    </row>
+    <row r="33" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="53" t="s">
+      <c r="C33" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="80"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="86" t="s">
+      <c r="D33" s="74"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+    </row>
+    <row r="34" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="53" t="s">
+      <c r="C34" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="80"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="86" t="s">
+      <c r="D34" s="74"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+    </row>
+    <row r="35" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="64" t="s">
+      <c r="C35" s="71"/>
+      <c r="D35" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="E35" s="58" t="s">
+      <c r="E35" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="86" t="s">
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+    </row>
+    <row r="36" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="64" t="s">
+      <c r="C36" s="71"/>
+      <c r="D36" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="E36" s="58" t="s">
+      <c r="E36" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58" t="s">
+      <c r="F36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="I36" s="58" t="s">
+      <c r="I36" s="71" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" s="86" t="s">
+    <row r="37" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="64" t="s">
+      <c r="C37" s="71"/>
+      <c r="D37" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="E37" s="58" t="s">
+      <c r="E37" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="86" t="s">
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="71"/>
+    </row>
+    <row r="38" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="64" t="s">
+      <c r="C38" s="71"/>
+      <c r="D38" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="E38" s="58" t="s">
+      <c r="E38" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B39" s="86" t="s">
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="71"/>
+    </row>
+    <row r="39" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="53"/>
-      <c r="D39" s="64" t="s">
+      <c r="C39" s="71"/>
+      <c r="D39" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="E39" s="58" t="s">
+      <c r="E39" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="64" t="s">
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="I39" s="58" t="s">
+      <c r="I39" s="71" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="86" t="s">
+    <row r="40" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="53"/>
-      <c r="D40" s="90" t="s">
+      <c r="C40" s="71"/>
+      <c r="D40" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="30" t="s">
+      <c r="E40" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="86" t="s">
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="71"/>
+    </row>
+    <row r="41" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="53"/>
-      <c r="D41" s="90" t="s">
+      <c r="C41" s="71"/>
+      <c r="D41" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="30" t="s">
+      <c r="E41" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="86" t="s">
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+    </row>
+    <row r="42" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="53"/>
-      <c r="D42" s="90" t="s">
+      <c r="C42" s="71"/>
+      <c r="D42" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="30" t="s">
+      <c r="E42" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30" t="s">
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="I42" s="30" t="s">
+      <c r="I42" s="71" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43" s="86" t="s">
+    <row r="43" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="53"/>
-      <c r="D43" s="81" t="s">
+      <c r="C43" s="71"/>
+      <c r="D43" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="E43" s="30" t="s">
+      <c r="E43" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="31" t="s">
+      <c r="F43" s="71"/>
+      <c r="G43" s="71"/>
+      <c r="H43" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="I43" s="30" t="s">
+      <c r="I43" s="71" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="59" t="s">
+      <c r="A44" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="33" t="s">
         <v>85</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="82"/>
+      <c r="D44" s="38"/>
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
@@ -3733,16 +3699,16 @@
       <c r="I44" s="14"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="59" t="s">
+      <c r="A45" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="33" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="82"/>
+      <c r="D45" s="38"/>
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
@@ -3753,378 +3719,380 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="87" t="s">
+    <row r="46" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B47" s="87" t="s">
+      <c r="D46" s="77"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="76"/>
+      <c r="H46" s="76"/>
+      <c r="I46" s="76"/>
+    </row>
+    <row r="47" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="83" t="s">
+      <c r="C47" s="76"/>
+      <c r="D47" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="E47" s="56" t="s">
+      <c r="E47" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B48" s="87" t="s">
+      <c r="F47" s="76"/>
+      <c r="G47" s="76"/>
+      <c r="H47" s="76"/>
+      <c r="I47" s="76"/>
+    </row>
+    <row r="48" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="84" t="s">
+      <c r="C48" s="76"/>
+      <c r="D48" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="56" t="s">
+      <c r="E48" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="56"/>
-      <c r="I48" s="56"/>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" s="87" t="s">
+      <c r="F48" s="76"/>
+      <c r="G48" s="76"/>
+      <c r="H48" s="76"/>
+      <c r="I48" s="76"/>
+    </row>
+    <row r="49" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="84" t="s">
+      <c r="C49" s="76"/>
+      <c r="D49" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="E49" s="56" t="s">
+      <c r="E49" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="56"/>
-      <c r="I49" s="56"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" s="87" t="s">
+      <c r="F49" s="76"/>
+      <c r="G49" s="76"/>
+      <c r="H49" s="76"/>
+      <c r="I49" s="76"/>
+    </row>
+    <row r="50" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="84" t="s">
+      <c r="C50" s="76"/>
+      <c r="D50" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="E50" s="56" t="s">
+      <c r="E50" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="F50" s="56"/>
-      <c r="G50" s="56"/>
-      <c r="H50" s="56" t="s">
+      <c r="F50" s="76"/>
+      <c r="G50" s="76"/>
+      <c r="H50" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="I50" s="56" t="s">
+      <c r="I50" s="76" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B51" s="87" t="s">
+    <row r="51" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="41" t="s">
+      <c r="C51" s="76"/>
+      <c r="D51" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="E51" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B52" s="87" t="s">
+      <c r="F51" s="76"/>
+      <c r="G51" s="76"/>
+      <c r="H51" s="76"/>
+      <c r="I51" s="76"/>
+    </row>
+    <row r="52" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="41" t="s">
+      <c r="C52" s="76"/>
+      <c r="D52" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E52" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B53" s="87" t="s">
+      <c r="F52" s="76"/>
+      <c r="G52" s="76"/>
+      <c r="H52" s="76"/>
+      <c r="I52" s="76"/>
+    </row>
+    <row r="53" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="84" t="s">
+      <c r="C53" s="76"/>
+      <c r="D53" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="E53" s="66" t="s">
+      <c r="E53" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="F53" s="43"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15" t="s">
+      <c r="F53" s="76"/>
+      <c r="G53" s="76"/>
+      <c r="H53" s="76"/>
+      <c r="I53" s="76" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" s="82" t="s">
+    <row r="54" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="42"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B55" s="82" t="s">
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+    </row>
+    <row r="55" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D55" s="84"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B56" s="82" t="s">
+      <c r="D55" s="16"/>
+      <c r="E55" s="80"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D56" s="84"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B57" s="82" t="s">
+      <c r="D56" s="16"/>
+      <c r="E56" s="80"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+    </row>
+    <row r="57" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D57" s="84"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14" t="s">
+      <c r="D57" s="16"/>
+      <c r="E57" s="80"/>
+      <c r="F57" s="81"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="I57" s="14" t="s">
+      <c r="I57" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B58" s="82" t="s">
+    <row r="58" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D58" s="84"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14" t="s">
+      <c r="D58" s="16"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="81"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="I58" s="14" t="s">
+      <c r="I58" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" s="84" t="s">
+    <row r="59" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="C59" s="43" t="s">
+      <c r="C59" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="D59" s="42"/>
-      <c r="E59" s="42"/>
-      <c r="F59" s="69"/>
-      <c r="G59" s="43"/>
-      <c r="H59" s="43"/>
-      <c r="I59" s="43"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B60" s="84" t="s">
+      <c r="D59" s="85"/>
+      <c r="E59" s="85"/>
+      <c r="F59" s="86"/>
+      <c r="G59" s="84"/>
+      <c r="H59" s="84"/>
+      <c r="I59" s="84"/>
+    </row>
+    <row r="60" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="71" t="s">
+      <c r="C60" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="D60" s="70"/>
-      <c r="E60" s="42"/>
-      <c r="F60" s="45"/>
-      <c r="G60" s="70"/>
-      <c r="H60" s="70"/>
-      <c r="I60" s="70"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B61" s="84" t="s">
+      <c r="D60" s="89"/>
+      <c r="E60" s="85"/>
+      <c r="F60" s="90"/>
+      <c r="G60" s="89"/>
+      <c r="H60" s="89"/>
+      <c r="I60" s="89"/>
+    </row>
+    <row r="61" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="C61" s="43" t="s">
+      <c r="C61" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="D61" s="84"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="43"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B62" s="84" t="s">
+      <c r="D61" s="83"/>
+      <c r="E61" s="85"/>
+      <c r="F61" s="84"/>
+      <c r="G61" s="84"/>
+      <c r="H61" s="84"/>
+      <c r="I61" s="84"/>
+    </row>
+    <row r="62" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="C62" s="43" t="s">
+      <c r="C62" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="D62" s="84"/>
-      <c r="E62" s="42"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
-      <c r="H62" s="43" t="s">
+      <c r="D62" s="83"/>
+      <c r="E62" s="85"/>
+      <c r="F62" s="84"/>
+      <c r="G62" s="84"/>
+      <c r="H62" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="I62" s="43" t="s">
+      <c r="I62" s="84" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B63" s="84" t="s">
+    <row r="63" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="C63" s="43" t="s">
+      <c r="C63" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="D63" s="84"/>
-      <c r="E63" s="42"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43" t="s">
+      <c r="D63" s="83"/>
+      <c r="E63" s="85"/>
+      <c r="F63" s="84"/>
+      <c r="G63" s="84"/>
+      <c r="H63" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="I63" s="43" t="s">
+      <c r="I63" s="84" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B64" s="84" t="s">
+    <row r="64" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="C64" s="43" t="s">
+      <c r="C64" s="84" t="s">
         <v>101</v>
       </c>
-      <c r="D64" s="84"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
-      <c r="H64" s="43" t="s">
+      <c r="D64" s="83"/>
+      <c r="E64" s="84"/>
+      <c r="F64" s="84"/>
+      <c r="G64" s="84"/>
+      <c r="H64" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="I64" s="43" t="s">
+      <c r="I64" s="84" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B65" s="17" t="s">
+      <c r="A65" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C65" s="15"/>
-      <c r="D65" s="17"/>
+      <c r="C65" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" s="16"/>
       <c r="E65" s="15"/>
       <c r="F65" s="15"/>
       <c r="G65" s="15"/>
@@ -4136,14 +4104,16 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B66" s="17" t="s">
+      <c r="A66" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="17"/>
+      <c r="C66" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" s="16"/>
       <c r="E66" s="15"/>
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
@@ -4155,42 +4125,42 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B67" s="17" t="s">
+      <c r="A67" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="17" t="s">
+      <c r="C67" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17" t="s">
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B68" s="17" t="s">
+      <c r="A68" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C68" s="17" t="s">
+      <c r="C68" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17" t="s">
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="17" t="s">
+      <c r="I68" s="16" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Guion y esqueleto 1 de los grados 8 y 9
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="107">
   <si>
     <t>FICHA</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>CS_08_01_CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1008,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1094,7 +1097,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1110,19 +1112,12 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1132,7 +1127,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1148,10 +1142,6 @@
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1173,6 +1163,20 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2823,10 +2827,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3087,7 +3091,7 @@
         <v>70</v>
       </c>
       <c r="C13" s="47"/>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="40" t="s">
         <v>72</v>
       </c>
       <c r="E13" s="44" t="s">
@@ -3106,7 +3110,7 @@
         <v>70</v>
       </c>
       <c r="C14" s="47"/>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="40" t="s">
         <v>72</v>
       </c>
       <c r="E14" s="44" t="s">
@@ -3125,7 +3129,7 @@
         <v>70</v>
       </c>
       <c r="C15" s="47"/>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="40" t="s">
         <v>72</v>
       </c>
       <c r="E15" s="44" t="s">
@@ -3144,7 +3148,7 @@
         <v>70</v>
       </c>
       <c r="C16" s="47"/>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="40" t="s">
         <v>72</v>
       </c>
       <c r="E16" s="44" t="s">
@@ -3166,213 +3170,214 @@
       <c r="B17" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="50" t="s">
+      <c r="C17" s="47"/>
+      <c r="D17" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="49" t="s">
+      <c r="E18" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="46" t="s">
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="I17" s="49" t="s">
+      <c r="I18" s="48" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="61" t="s">
+    <row r="19" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C19" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="63"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
-    </row>
-    <row r="19" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="61" t="s">
+      <c r="D19" s="84"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+    </row>
+    <row r="20" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C20" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="65"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-    </row>
-    <row r="20" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="61" t="s">
+      <c r="D20" s="61"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
+    </row>
+    <row r="21" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="62" t="s">
+      <c r="C21" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="65"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-    </row>
-    <row r="21" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="61" t="s">
+      <c r="D21" s="61"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+    </row>
+    <row r="22" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="62" t="s">
+      <c r="C22" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="65"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62" t="s">
+      <c r="D22" s="61"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="I21" s="62" t="s">
+      <c r="I22" s="59" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="61" t="s">
+    <row r="23" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C23" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="67"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="I22" s="68"/>
-    </row>
-    <row r="23" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="61" t="s">
+      <c r="D23" s="63"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+    </row>
+    <row r="24" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="62" t="s">
+      <c r="C24" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="63"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+    </row>
+    <row r="25" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="59"/>
+      <c r="D25" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="67"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62" t="s">
+      <c r="E25" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="62" t="s">
+      <c r="I25" s="59" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-    </row>
-    <row r="25" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-    </row>
-    <row r="26" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
+    <row r="26" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="32" t="s">
+      <c r="C26" s="32" t="s">
         <v>24</v>
       </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="32"/>
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
     </row>
-    <row r="27" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
+    <row r="27" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="32" t="s">
-        <v>30</v>
-      </c>
+      <c r="C27" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="37"/>
+      <c r="E27" s="32"/>
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
       <c r="H27" s="32"/>
       <c r="I27" s="32"/>
     </row>
-    <row r="28" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="53" t="s">
+    <row r="28" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="35" t="s">
         <v>76</v>
       </c>
       <c r="C28" s="32"/>
-      <c r="D28" s="56" t="s">
-        <v>78</v>
+      <c r="D28" s="54" t="s">
+        <v>77</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>24</v>
@@ -3382,785 +3387,905 @@
       <c r="H28" s="32"/>
       <c r="I28" s="32"/>
     </row>
-    <row r="29" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="53" t="s">
+    <row r="29" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B29" s="35" t="s">
         <v>76</v>
       </c>
       <c r="C29" s="32"/>
-      <c r="D29" s="56" t="s">
-        <v>78</v>
+      <c r="D29" s="54" t="s">
+        <v>77</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F29" s="32"/>
       <c r="G29" s="32"/>
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
     </row>
-    <row r="30" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
+    <row r="30" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="35" t="s">
         <v>76</v>
       </c>
       <c r="C30" s="32"/>
-      <c r="D30" s="56" t="s">
+      <c r="D30" s="55" t="s">
         <v>78</v>
       </c>
       <c r="E30" s="32" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F30" s="32"/>
       <c r="G30" s="32"/>
       <c r="H30" s="32"/>
       <c r="I30" s="32"/>
     </row>
-    <row r="31" spans="1:9" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="53" t="s">
+    <row r="31" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="35" t="s">
         <v>76</v>
       </c>
       <c r="C31" s="32"/>
-      <c r="D31" s="57" t="s">
-        <v>100</v>
-      </c>
-      <c r="E31" s="58" t="s">
-        <v>29</v>
+      <c r="D31" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>25</v>
       </c>
       <c r="F31" s="32"/>
       <c r="G31" s="32"/>
-      <c r="H31" s="59" t="s">
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+    </row>
+    <row r="32" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="32"/>
+      <c r="D32" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+    </row>
+    <row r="33" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="32"/>
+      <c r="D33" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+    </row>
+    <row r="34" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="32"/>
+      <c r="D34" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="87" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="I31" s="32" t="s">
+      <c r="I34" s="32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="70" t="s">
+    <row r="35" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="71" t="s">
+      <c r="C35" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="72"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="71"/>
-    </row>
-    <row r="33" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="70" t="s">
+      <c r="D35" s="67"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="66"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
+    </row>
+    <row r="36" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="71" t="s">
+      <c r="C36" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="74"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="71"/>
-    </row>
-    <row r="34" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="70" t="s">
+      <c r="D36" s="69"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="66"/>
+    </row>
+    <row r="37" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="71" t="s">
+      <c r="C37" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
-    </row>
-    <row r="35" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="70" t="s">
+      <c r="D37" s="69"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="66"/>
+    </row>
+    <row r="38" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="71"/>
-      <c r="D35" s="74" t="s">
+      <c r="C38" s="66"/>
+      <c r="D38" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="E35" s="71" t="s">
+      <c r="E38" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="71"/>
-    </row>
-    <row r="36" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="70" t="s">
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="66"/>
+    </row>
+    <row r="39" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="74" t="s">
+      <c r="C39" s="66"/>
+      <c r="D39" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="E36" s="71" t="s">
+      <c r="E39" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="71"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="71" t="s">
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="I36" s="71" t="s">
+      <c r="I39" s="66" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" s="70" t="s">
+    <row r="40" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="71"/>
-      <c r="D37" s="74" t="s">
+      <c r="C40" s="66"/>
+      <c r="D40" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="E37" s="71" t="s">
+      <c r="E40" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="F37" s="71"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="71"/>
-    </row>
-    <row r="38" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="70" t="s">
+      <c r="F40" s="66"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="66"/>
+    </row>
+    <row r="41" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="71"/>
-      <c r="D38" s="74" t="s">
+      <c r="C41" s="66"/>
+      <c r="D41" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="E38" s="71" t="s">
+      <c r="E41" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="71"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="71"/>
-      <c r="I38" s="71"/>
-    </row>
-    <row r="39" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B39" s="70" t="s">
+      <c r="F41" s="66"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="66"/>
+      <c r="I41" s="66"/>
+    </row>
+    <row r="42" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="71"/>
-      <c r="D39" s="74" t="s">
+      <c r="C42" s="66"/>
+      <c r="D42" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="E39" s="71" t="s">
+      <c r="E42" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="71"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="74" t="s">
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="I39" s="71" t="s">
+      <c r="I42" s="66" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="70" t="s">
+    <row r="43" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="71"/>
-      <c r="D40" s="70" t="s">
+      <c r="C43" s="66"/>
+      <c r="D43" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="71" t="s">
+      <c r="E43" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="F40" s="71"/>
-      <c r="G40" s="71"/>
-      <c r="H40" s="71"/>
-      <c r="I40" s="71"/>
-    </row>
-    <row r="41" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="70" t="s">
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+    </row>
+    <row r="44" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="70" t="s">
+      <c r="C44" s="66"/>
+      <c r="D44" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="71" t="s">
+      <c r="E44" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="71"/>
-      <c r="G41" s="71"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
-    </row>
-    <row r="42" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="70" t="s">
+      <c r="F44" s="66"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="66"/>
+    </row>
+    <row r="45" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="71"/>
-      <c r="D42" s="70" t="s">
+      <c r="C45" s="66"/>
+      <c r="D45" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="71" t="s">
+      <c r="E45" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="F42" s="71"/>
-      <c r="G42" s="71"/>
-      <c r="H42" s="71" t="s">
+      <c r="F45" s="66"/>
+      <c r="G45" s="66"/>
+      <c r="H45" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="I42" s="71" t="s">
+      <c r="I45" s="66" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43" s="70" t="s">
+    <row r="46" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="71"/>
-      <c r="D43" s="74" t="s">
+      <c r="C46" s="66"/>
+      <c r="D46" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="66"/>
+      <c r="G46" s="66"/>
+      <c r="H46" s="86"/>
+      <c r="I46" s="66"/>
+    </row>
+    <row r="47" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="66"/>
+      <c r="D47" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="E43" s="71" t="s">
+      <c r="E47" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="71"/>
-      <c r="G43" s="71"/>
-      <c r="H43" s="75" t="s">
+      <c r="F47" s="66"/>
+      <c r="G47" s="66"/>
+      <c r="H47" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="I43" s="71" t="s">
+      <c r="I47" s="66" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="33" t="s">
+    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C48" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="38"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="33" t="s">
+      <c r="D48" s="38"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C49" s="14"/>
+      <c r="D49" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="38"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14" t="s">
+      <c r="E49" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="I45" s="14" t="s">
+      <c r="I49" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="70" t="s">
+    <row r="50" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="76" t="s">
+      <c r="C50" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="77"/>
-      <c r="E46" s="76"/>
-      <c r="F46" s="76"/>
-      <c r="G46" s="76"/>
-      <c r="H46" s="76"/>
-      <c r="I46" s="76"/>
-    </row>
-    <row r="47" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B47" s="70" t="s">
+      <c r="D50" s="72"/>
+      <c r="E50" s="71"/>
+      <c r="F50" s="71"/>
+      <c r="G50" s="71"/>
+      <c r="H50" s="71"/>
+      <c r="I50" s="71"/>
+    </row>
+    <row r="51" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="76"/>
-      <c r="D47" s="77" t="s">
+      <c r="C51" s="71"/>
+      <c r="D51" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="E47" s="76" t="s">
+      <c r="E51" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="F47" s="76"/>
-      <c r="G47" s="76"/>
-      <c r="H47" s="76"/>
-      <c r="I47" s="76"/>
-    </row>
-    <row r="48" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B48" s="70" t="s">
+      <c r="F51" s="71"/>
+      <c r="G51" s="71"/>
+      <c r="H51" s="71"/>
+      <c r="I51" s="71"/>
+    </row>
+    <row r="52" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="76"/>
-      <c r="D48" s="77" t="s">
+      <c r="C52" s="71"/>
+      <c r="D52" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="76" t="s">
+      <c r="E52" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="F48" s="76"/>
-      <c r="G48" s="76"/>
-      <c r="H48" s="76"/>
-      <c r="I48" s="76"/>
-    </row>
-    <row r="49" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" s="70" t="s">
+      <c r="F52" s="71"/>
+      <c r="G52" s="71"/>
+      <c r="H52" s="71"/>
+      <c r="I52" s="71"/>
+    </row>
+    <row r="53" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="76"/>
-      <c r="D49" s="77" t="s">
+      <c r="C53" s="71"/>
+      <c r="D53" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="E49" s="76" t="s">
+      <c r="E53" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="F49" s="76"/>
-      <c r="G49" s="76"/>
-      <c r="H49" s="76"/>
-      <c r="I49" s="76"/>
-    </row>
-    <row r="50" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" s="70" t="s">
+      <c r="F53" s="71"/>
+      <c r="G53" s="71"/>
+      <c r="H53" s="71"/>
+      <c r="I53" s="71"/>
+    </row>
+    <row r="54" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="76"/>
-      <c r="D50" s="77" t="s">
+      <c r="C54" s="71"/>
+      <c r="D54" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="E50" s="76" t="s">
+      <c r="E54" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="F50" s="76"/>
-      <c r="G50" s="76"/>
-      <c r="H50" s="76" t="s">
+      <c r="F54" s="71"/>
+      <c r="G54" s="71"/>
+      <c r="H54" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="I50" s="76" t="s">
+      <c r="I54" s="71" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B51" s="70" t="s">
+    <row r="55" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="76"/>
-      <c r="D51" s="78" t="s">
+      <c r="C55" s="71"/>
+      <c r="D55" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="E51" s="76" t="s">
+      <c r="E55" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="F51" s="76"/>
-      <c r="G51" s="76"/>
-      <c r="H51" s="76"/>
-      <c r="I51" s="76"/>
-    </row>
-    <row r="52" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B52" s="70" t="s">
+      <c r="F55" s="71"/>
+      <c r="G55" s="71"/>
+      <c r="H55" s="71"/>
+      <c r="I55" s="71"/>
+    </row>
+    <row r="56" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="76"/>
-      <c r="D52" s="78" t="s">
+      <c r="C56" s="71"/>
+      <c r="D56" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="E56" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="71"/>
+      <c r="G56" s="71"/>
+      <c r="H56" s="71"/>
+      <c r="I56" s="71"/>
+    </row>
+    <row r="57" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" s="65" t="s">
+        <v>102</v>
+      </c>
+      <c r="C57" s="71"/>
+      <c r="D57" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="E52" s="76" t="s">
-        <v>27</v>
-      </c>
-      <c r="F52" s="76"/>
-      <c r="G52" s="76"/>
-      <c r="H52" s="76"/>
-      <c r="I52" s="76"/>
-    </row>
-    <row r="53" spans="1:9" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B53" s="70" t="s">
+      <c r="E57" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="71"/>
+      <c r="G57" s="71"/>
+      <c r="H57" s="71"/>
+      <c r="I57" s="71"/>
+    </row>
+    <row r="58" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="76"/>
-      <c r="D53" s="77" t="s">
+      <c r="C58" s="71"/>
+      <c r="D58" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="E53" s="79" t="s">
+      <c r="E58" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="F53" s="76"/>
-      <c r="G53" s="76"/>
-      <c r="H53" s="76"/>
-      <c r="I53" s="76" t="s">
+      <c r="F58" s="71"/>
+      <c r="G58" s="71"/>
+      <c r="H58" s="71"/>
+      <c r="I58" s="71" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" s="16" t="s">
+    <row r="59" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C59" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="80"/>
-      <c r="E54" s="80"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-    </row>
-    <row r="55" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="B55" s="16" t="s">
+      <c r="D59" s="73"/>
+      <c r="E59" s="73"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C60" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D55" s="16"/>
-      <c r="E55" s="80"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-    </row>
-    <row r="56" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="B56" s="16" t="s">
+      <c r="D60" s="16"/>
+      <c r="E60" s="73"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+    </row>
+    <row r="61" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C61" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D56" s="16"/>
-      <c r="E56" s="80"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="15"/>
-    </row>
-    <row r="57" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="B57" s="16" t="s">
+      <c r="D61" s="16"/>
+      <c r="E61" s="73"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+    </row>
+    <row r="62" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C62" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="80"/>
-      <c r="F57" s="81"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15" t="s">
+      <c r="D62" s="16"/>
+      <c r="E62" s="73"/>
+      <c r="F62" s="74"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="I57" s="15" t="s">
+      <c r="I62" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="B58" s="16" t="s">
+    <row r="63" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C63" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D63" s="16"/>
+      <c r="E63" s="73"/>
+      <c r="F63" s="74"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+    </row>
+    <row r="64" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F64" s="74"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I64" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="C65" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="78"/>
+      <c r="E65" s="78"/>
+      <c r="F65" s="79"/>
+      <c r="G65" s="77"/>
+      <c r="H65" s="77"/>
+      <c r="I65" s="77"/>
+    </row>
+    <row r="66" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="C66" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="D66" s="82"/>
+      <c r="E66" s="78"/>
+      <c r="F66" s="83"/>
+      <c r="G66" s="82"/>
+      <c r="H66" s="82"/>
+      <c r="I66" s="82"/>
+    </row>
+    <row r="67" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="C67" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67" s="76"/>
+      <c r="E67" s="78"/>
+      <c r="F67" s="77"/>
+      <c r="G67" s="77"/>
+      <c r="H67" s="77"/>
+      <c r="I67" s="77"/>
+    </row>
+    <row r="68" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="C68" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="76"/>
+      <c r="E68" s="78"/>
+      <c r="F68" s="77"/>
+      <c r="G68" s="77"/>
+      <c r="H68" s="77" t="s">
+        <v>93</v>
+      </c>
+      <c r="I68" s="77" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="C69" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" s="76"/>
+      <c r="E69" s="78"/>
+      <c r="F69" s="77"/>
+      <c r="G69" s="77"/>
+      <c r="H69" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="I69" s="77" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" s="77"/>
+      <c r="D70" s="76" t="s">
         <v>101</v>
       </c>
-      <c r="D58" s="16"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="81"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="I58" s="15" t="s">
+      <c r="E70" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="F70" s="77"/>
+      <c r="G70" s="77"/>
+      <c r="H70" s="77" t="s">
+        <v>94</v>
+      </c>
+      <c r="I70" s="77" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="82" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="C59" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="D59" s="85"/>
-      <c r="E59" s="85"/>
-      <c r="F59" s="86"/>
-      <c r="G59" s="84"/>
-      <c r="H59" s="84"/>
-      <c r="I59" s="84"/>
-    </row>
-    <row r="60" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="82" t="s">
-        <v>31</v>
-      </c>
-      <c r="B60" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="C60" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="D60" s="89"/>
-      <c r="E60" s="85"/>
-      <c r="F60" s="90"/>
-      <c r="G60" s="89"/>
-      <c r="H60" s="89"/>
-      <c r="I60" s="89"/>
-    </row>
-    <row r="61" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="82" t="s">
-        <v>31</v>
-      </c>
-      <c r="B61" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="C61" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="D61" s="83"/>
-      <c r="E61" s="85"/>
-      <c r="F61" s="84"/>
-      <c r="G61" s="84"/>
-      <c r="H61" s="84"/>
-      <c r="I61" s="84"/>
-    </row>
-    <row r="62" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="82" t="s">
-        <v>31</v>
-      </c>
-      <c r="B62" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="C62" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D62" s="83"/>
-      <c r="E62" s="85"/>
-      <c r="F62" s="84"/>
-      <c r="G62" s="84"/>
-      <c r="H62" s="84" t="s">
-        <v>93</v>
-      </c>
-      <c r="I62" s="84" t="s">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D71" s="16"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I71" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="82" t="s">
-        <v>31</v>
-      </c>
-      <c r="B63" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="C63" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D63" s="83"/>
-      <c r="E63" s="85"/>
-      <c r="F63" s="84"/>
-      <c r="G63" s="84"/>
-      <c r="H63" s="84" t="s">
-        <v>92</v>
-      </c>
-      <c r="I63" s="84" t="s">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" s="16"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I72" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="82" t="s">
-        <v>31</v>
-      </c>
-      <c r="B64" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="C64" s="84" t="s">
-        <v>101</v>
-      </c>
-      <c r="D64" s="83"/>
-      <c r="E64" s="84"/>
-      <c r="F64" s="84"/>
-      <c r="G64" s="84"/>
-      <c r="H64" s="84" t="s">
-        <v>94</v>
-      </c>
-      <c r="I64" s="84" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D65" s="16"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="I65" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B66" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D66" s="16"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="I66" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B67" s="16" t="s">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="C73" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
-      <c r="I67" s="16" t="s">
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B68" s="16" t="s">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="C74" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16" t="s">
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="16" t="s">
+      <c r="I74" s="16" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Guion y esqueleto 1 grado 8_Final
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="5955" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -15,18 +15,18 @@
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="106">
   <si>
     <t>FICHA</t>
   </si>
@@ -338,9 +338,6 @@
   </si>
   <si>
     <t xml:space="preserve"> El contexto político de la Ilustración</t>
-  </si>
-  <si>
-    <t>La Revolución inglesa de 1689</t>
   </si>
   <si>
     <t>CS_08_01_CO</t>
@@ -1139,7 +1136,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1167,9 +1163,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1177,6 +1170,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1849,7 +1844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1882,7 +1877,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2454,7 +2449,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D39"/>
@@ -2827,10 +2822,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3172,7 +3167,7 @@
       </c>
       <c r="C17" s="47"/>
       <c r="D17" s="40" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>24</v>
@@ -3215,7 +3210,7 @@
       <c r="C19" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="84"/>
+      <c r="D19" s="83"/>
       <c r="E19" s="59"/>
       <c r="F19" s="59"/>
       <c r="G19" s="59"/>
@@ -3291,8 +3286,8 @@
       <c r="E23" s="59"/>
       <c r="F23" s="59"/>
       <c r="G23" s="59"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="85"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="84"/>
     </row>
     <row r="24" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="62" t="s">
@@ -3301,15 +3296,17 @@
       <c r="B24" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="59" t="s">
+      <c r="C24" s="59"/>
+      <c r="D24" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="63"/>
-      <c r="E24" s="59"/>
       <c r="F24" s="59"/>
       <c r="G24" s="59"/>
-      <c r="H24" s="85"/>
-      <c r="I24" s="85"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="84"/>
     </row>
     <row r="25" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="62" t="s">
@@ -3472,7 +3469,7 @@
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="55" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="E33" s="32" t="s">
         <v>24</v>
@@ -3493,12 +3490,12 @@
       <c r="D34" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="87" t="s">
+      <c r="E34" s="85" t="s">
         <v>29</v>
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="32"/>
-      <c r="H34" s="89" t="s">
+      <c r="H34" s="87" t="s">
         <v>81</v>
       </c>
       <c r="I34" s="32" t="s">
@@ -3729,14 +3726,14 @@
       </c>
       <c r="C46" s="66"/>
       <c r="D46" s="65" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="E46" s="66" t="s">
         <v>24</v>
       </c>
       <c r="F46" s="66"/>
       <c r="G46" s="66"/>
-      <c r="H46" s="86"/>
+      <c r="H46" s="66"/>
       <c r="I46" s="66"/>
     </row>
     <row r="47" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3755,7 +3752,7 @@
       </c>
       <c r="F47" s="66"/>
       <c r="G47" s="66"/>
-      <c r="H47" s="70" t="s">
+      <c r="H47" s="88" t="s">
         <v>84</v>
       </c>
       <c r="I47" s="66" t="s">
@@ -3788,36 +3785,38 @@
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F49" s="14"/>
       <c r="G49" s="14"/>
-      <c r="H49" s="14" t="s">
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="I49" s="14" t="s">
+      <c r="I50" s="14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" s="65" t="s">
-        <v>102</v>
-      </c>
-      <c r="C50" s="71" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" s="72"/>
-      <c r="E50" s="71"/>
-      <c r="F50" s="71"/>
-      <c r="G50" s="71"/>
-      <c r="H50" s="71"/>
-      <c r="I50" s="71"/>
     </row>
     <row r="51" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="64" t="s">
@@ -3826,17 +3825,15 @@
       <c r="B51" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="71"/>
-      <c r="D51" s="72" t="s">
-        <v>87</v>
-      </c>
-      <c r="E51" s="71" t="s">
+      <c r="C51" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="F51" s="71"/>
-      <c r="G51" s="71"/>
-      <c r="H51" s="71"/>
-      <c r="I51" s="71"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="70"/>
+      <c r="F51" s="70"/>
+      <c r="G51" s="70"/>
+      <c r="H51" s="70"/>
+      <c r="I51" s="70"/>
     </row>
     <row r="52" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="64" t="s">
@@ -3845,17 +3842,17 @@
       <c r="B52" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="71"/>
-      <c r="D52" s="72" t="s">
+      <c r="C52" s="70"/>
+      <c r="D52" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E52" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" s="71"/>
-      <c r="G52" s="71"/>
-      <c r="H52" s="71"/>
-      <c r="I52" s="71"/>
+      <c r="E52" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="70"/>
+      <c r="G52" s="70"/>
+      <c r="H52" s="70"/>
+      <c r="I52" s="70"/>
     </row>
     <row r="53" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="64" t="s">
@@ -3864,17 +3861,17 @@
       <c r="B53" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="71"/>
-      <c r="D53" s="72" t="s">
+      <c r="C53" s="70"/>
+      <c r="D53" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E53" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="F53" s="71"/>
-      <c r="G53" s="71"/>
-      <c r="H53" s="71"/>
-      <c r="I53" s="71"/>
+      <c r="E53" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="70"/>
+      <c r="G53" s="70"/>
+      <c r="H53" s="70"/>
+      <c r="I53" s="70"/>
     </row>
     <row r="54" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="64" t="s">
@@ -3883,21 +3880,17 @@
       <c r="B54" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="71"/>
-      <c r="D54" s="72" t="s">
+      <c r="C54" s="70"/>
+      <c r="D54" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E54" s="71" t="s">
-        <v>29</v>
-      </c>
-      <c r="F54" s="71"/>
-      <c r="G54" s="71"/>
-      <c r="H54" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="I54" s="71" t="s">
-        <v>21</v>
-      </c>
+      <c r="E54" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="70"/>
+      <c r="G54" s="70"/>
+      <c r="H54" s="70"/>
+      <c r="I54" s="70"/>
     </row>
     <row r="55" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="64" t="s">
@@ -3906,17 +3899,17 @@
       <c r="B55" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="71"/>
-      <c r="D55" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="E55" s="71" t="s">
-        <v>24</v>
-      </c>
-      <c r="F55" s="71"/>
-      <c r="G55" s="71"/>
-      <c r="H55" s="71"/>
-      <c r="I55" s="71"/>
+      <c r="C55" s="70"/>
+      <c r="D55" s="71" t="s">
+        <v>87</v>
+      </c>
+      <c r="E55" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="F55" s="70"/>
+      <c r="G55" s="70"/>
+      <c r="H55" s="70"/>
+      <c r="I55" s="70"/>
     </row>
     <row r="56" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="64" t="s">
@@ -3925,17 +3918,21 @@
       <c r="B56" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C56" s="71"/>
-      <c r="D56" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="E56" s="71" t="s">
-        <v>27</v>
-      </c>
-      <c r="F56" s="71"/>
-      <c r="G56" s="71"/>
-      <c r="H56" s="71"/>
-      <c r="I56" s="71"/>
+      <c r="C56" s="70"/>
+      <c r="D56" s="71" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="F56" s="70"/>
+      <c r="G56" s="70"/>
+      <c r="H56" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="I56" s="70" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="57" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="64" t="s">
@@ -3944,17 +3941,17 @@
       <c r="B57" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="71"/>
+      <c r="C57" s="70"/>
       <c r="D57" s="65" t="s">
-        <v>104</v>
-      </c>
-      <c r="E57" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="E57" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="F57" s="71"/>
-      <c r="G57" s="71"/>
-      <c r="H57" s="71"/>
-      <c r="I57" s="71"/>
+      <c r="F57" s="70"/>
+      <c r="G57" s="70"/>
+      <c r="H57" s="70"/>
+      <c r="I57" s="70"/>
     </row>
     <row r="58" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="64" t="s">
@@ -3963,53 +3960,57 @@
       <c r="B58" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="C58" s="71"/>
-      <c r="D58" s="72" t="s">
+      <c r="C58" s="70"/>
+      <c r="D58" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="E58" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58" s="70"/>
+      <c r="G58" s="70"/>
+      <c r="H58" s="70"/>
+      <c r="I58" s="70"/>
+    </row>
+    <row r="59" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="65" t="s">
+        <v>102</v>
+      </c>
+      <c r="C59" s="70"/>
+      <c r="D59" s="65" t="s">
         <v>100</v>
       </c>
-      <c r="E58" s="88" t="s">
+      <c r="E59" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="70"/>
+      <c r="G59" s="70"/>
+      <c r="H59" s="70"/>
+      <c r="I59" s="70"/>
+    </row>
+    <row r="60" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="65" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" s="70"/>
+      <c r="D60" s="71" t="s">
+        <v>100</v>
+      </c>
+      <c r="E60" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="F58" s="71"/>
-      <c r="G58" s="71"/>
-      <c r="H58" s="71"/>
-      <c r="I58" s="71" t="s">
+      <c r="F60" s="70"/>
+      <c r="G60" s="70"/>
+      <c r="H60" s="70"/>
+      <c r="I60" s="70" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C59" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D59" s="73"/>
-      <c r="E59" s="73"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-    </row>
-    <row r="60" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D60" s="16"/>
-      <c r="E60" s="73"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
-      <c r="I60" s="15"/>
     </row>
     <row r="61" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="51" t="s">
@@ -4021,8 +4022,8 @@
       <c r="C61" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D61" s="16"/>
-      <c r="E61" s="73"/>
+      <c r="D61" s="72"/>
+      <c r="E61" s="72"/>
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
@@ -4036,18 +4037,14 @@
         <v>89</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D62" s="16"/>
-      <c r="E62" s="73"/>
-      <c r="F62" s="74"/>
+      <c r="E62" s="72"/>
+      <c r="F62" s="15"/>
       <c r="G62" s="15"/>
-      <c r="H62" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I62" s="15" t="s">
-        <v>20</v>
-      </c>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
     </row>
     <row r="63" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="51" t="s">
@@ -4060,8 +4057,8 @@
         <v>24</v>
       </c>
       <c r="D63" s="16"/>
-      <c r="E63" s="73"/>
-      <c r="F63" s="74"/>
+      <c r="E63" s="72"/>
+      <c r="F63" s="15"/>
       <c r="G63" s="15"/>
       <c r="H63" s="15"/>
       <c r="I63" s="15"/>
@@ -4074,218 +4071,294 @@
         <v>89</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D64" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E64" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F64" s="74"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="72"/>
+      <c r="F64" s="73"/>
       <c r="G64" s="15"/>
       <c r="H64" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I64" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="75" t="s">
-        <v>31</v>
-      </c>
-      <c r="B65" s="76" t="s">
+    <row r="65" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C65" s="15"/>
+      <c r="D65" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E65" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="F65" s="73"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+    </row>
+    <row r="66" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" s="73"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I66" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="C65" s="77" t="s">
+      <c r="C67" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="D65" s="78"/>
-      <c r="E65" s="78"/>
-      <c r="F65" s="79"/>
-      <c r="G65" s="77"/>
-      <c r="H65" s="77"/>
-      <c r="I65" s="77"/>
-    </row>
-    <row r="66" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="75" t="s">
-        <v>31</v>
-      </c>
-      <c r="B66" s="76" t="s">
+      <c r="D67" s="77"/>
+      <c r="E67" s="77"/>
+      <c r="F67" s="78"/>
+      <c r="G67" s="76"/>
+      <c r="H67" s="76"/>
+      <c r="I67" s="76"/>
+    </row>
+    <row r="68" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="C66" s="81" t="s">
+      <c r="C68" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="D66" s="82"/>
-      <c r="E66" s="78"/>
-      <c r="F66" s="83"/>
-      <c r="G66" s="82"/>
-      <c r="H66" s="82"/>
-      <c r="I66" s="82"/>
-    </row>
-    <row r="67" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="75" t="s">
-        <v>31</v>
-      </c>
-      <c r="B67" s="76" t="s">
+      <c r="D68" s="81"/>
+      <c r="E68" s="77"/>
+      <c r="F68" s="82"/>
+      <c r="G68" s="81"/>
+      <c r="H68" s="81"/>
+      <c r="I68" s="81"/>
+    </row>
+    <row r="69" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="C67" s="77" t="s">
+      <c r="C69" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="D67" s="76"/>
-      <c r="E67" s="78"/>
-      <c r="F67" s="77"/>
-      <c r="G67" s="77"/>
-      <c r="H67" s="77"/>
-      <c r="I67" s="77"/>
-    </row>
-    <row r="68" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="75" t="s">
-        <v>31</v>
-      </c>
-      <c r="B68" s="76" t="s">
+      <c r="D69" s="75"/>
+      <c r="E69" s="77"/>
+      <c r="F69" s="76"/>
+      <c r="G69" s="76"/>
+      <c r="H69" s="76"/>
+      <c r="I69" s="76"/>
+    </row>
+    <row r="70" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="C68" s="77" t="s">
+      <c r="C70" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="D68" s="76"/>
-      <c r="E68" s="78"/>
-      <c r="F68" s="77"/>
-      <c r="G68" s="77"/>
-      <c r="H68" s="77" t="s">
+      <c r="D70" s="75"/>
+      <c r="E70" s="77"/>
+      <c r="F70" s="76"/>
+      <c r="G70" s="76"/>
+      <c r="H70" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="I68" s="77" t="s">
+      <c r="I70" s="76" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="75" t="s">
-        <v>31</v>
-      </c>
-      <c r="B69" s="76" t="s">
+    <row r="71" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="C69" s="77" t="s">
+      <c r="C71" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="D69" s="76"/>
-      <c r="E69" s="78"/>
-      <c r="F69" s="77"/>
-      <c r="G69" s="77"/>
-      <c r="H69" s="77" t="s">
+      <c r="D71" s="75"/>
+      <c r="E71" s="77"/>
+      <c r="F71" s="76"/>
+      <c r="G71" s="76"/>
+      <c r="H71" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="I69" s="77" t="s">
+      <c r="I71" s="76" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="75" t="s">
-        <v>31</v>
-      </c>
-      <c r="B70" s="76" t="s">
+    <row r="72" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="C70" s="77"/>
-      <c r="D70" s="76" t="s">
+      <c r="C72" s="76"/>
+      <c r="D72" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="E70" s="77" t="s">
+      <c r="E72" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="F72" s="76"/>
+      <c r="G72" s="76"/>
+      <c r="H72" s="76"/>
+      <c r="I72" s="76"/>
+    </row>
+    <row r="73" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="C73" s="76"/>
+      <c r="D73" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="E73" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="F70" s="77"/>
-      <c r="G70" s="77"/>
-      <c r="H70" s="77" t="s">
+      <c r="F73" s="76"/>
+      <c r="G73" s="76"/>
+      <c r="H73" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="I70" s="77" t="s">
+      <c r="I73" s="76" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B71" s="16" t="s">
+    <row r="74" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C74" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D74" s="16"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C75" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D71" s="16"/>
-      <c r="E71" s="15"/>
-      <c r="F71" s="15"/>
-      <c r="G71" s="15"/>
-      <c r="H71" s="15" t="s">
+      <c r="D75" s="16"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="I71" s="15" t="s">
+      <c r="I75" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B72" s="16" t="s">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C72" s="15" t="s">
+      <c r="C76" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D72" s="16"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15" t="s">
+      <c r="D76" s="16"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="I72" s="15" t="s">
+      <c r="I76" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B73" s="16" t="s">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="C73" s="16" t="s">
+      <c r="C77" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="16"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="16"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="16"/>
-      <c r="I73" s="16" t="s">
+      <c r="D77" s="16"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="16"/>
+      <c r="I77" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B74" s="16" t="s">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C74" s="16" t="s">
+      <c r="C78" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="16"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="16" t="s">
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I74" s="16" t="s">
+      <c r="I78" s="16" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Guiones 1 y 2 de grado 9. Guion 1 de grado 8.
Incluye esqueletos y recursos.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
@@ -13,7 +13,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="106">
   <si>
     <t>FICHA</t>
   </si>
@@ -1844,7 +1844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2824,8 +2824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43:G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4336,7 +4336,9 @@
       <c r="E77" s="16"/>
       <c r="F77" s="16"/>
       <c r="G77" s="16"/>
-      <c r="H77" s="16"/>
+      <c r="H77" s="16" t="s">
+        <v>22</v>
+      </c>
       <c r="I77" s="16" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
CS0801: Ajuste de errores de nombres de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasSociales\fuentes\contenidos\grado08\guion01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="5955" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19082" windowHeight="5956" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="86">
   <si>
     <t>FICHA</t>
   </si>
@@ -127,9 +132,6 @@
     <t>¿Qué fue el Antiguo Régimen? ¿Cómo se produjo su fin? ¿Cuáles fueron las consecuencias de la difusión de las ideas ilustradas? Así comenzó la Edad Contemporánea.</t>
   </si>
   <si>
-    <t>4° ESO</t>
-  </si>
-  <si>
     <t>El absolutismo</t>
   </si>
   <si>
@@ -178,12 +180,6 @@
     <t>Refuerza tu aprendizaje: La crisis del Antiguo Régimen</t>
   </si>
   <si>
-    <t>5º ESO</t>
-  </si>
-  <si>
-    <t>6º ESO</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Las revoluciones inglesas</t>
   </si>
   <si>
@@ -208,30 +204,6 @@
     <t>Cronología: el fin del Antiguo Régimen</t>
   </si>
   <si>
-    <t>7º ESO</t>
-  </si>
-  <si>
-    <t>8º ESO</t>
-  </si>
-  <si>
-    <t>9º ESO</t>
-  </si>
-  <si>
-    <t>10º ESO</t>
-  </si>
-  <si>
-    <t>11º ESO</t>
-  </si>
-  <si>
-    <t>12º ESO</t>
-  </si>
-  <si>
-    <t>13º ESO</t>
-  </si>
-  <si>
-    <t>14º ESO</t>
-  </si>
-  <si>
     <t>El pensamiento ilustrado frente a la idea del poder divino</t>
   </si>
   <si>
@@ -247,12 +219,6 @@
     <t>El despotismo ilustrado</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: La ilustración.</t>
-  </si>
-  <si>
-    <t>Las ideas de la Ilustración.</t>
-  </si>
-  <si>
     <t>La sociedad del Antiguo Régimen</t>
   </si>
   <si>
@@ -280,15 +246,9 @@
     <t>El liberalismo político</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: el pensamiento liberal</t>
-  </si>
-  <si>
     <t>La crisis del antiguo régimen</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: la crisis del Antiguo Régimen </t>
-  </si>
-  <si>
     <t>La Guerra Civil</t>
   </si>
   <si>
@@ -298,25 +258,10 @@
     <t>La Revolución americana</t>
   </si>
   <si>
-    <t>Conoce la Revolución americana</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: La Revolución americana</t>
-  </si>
-  <si>
     <t>La Revolución francesa</t>
   </si>
   <si>
-    <t>La Declaración de los Derechos del Hombre y del Ciudadano</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: La Revolución francesa.</t>
-  </si>
-  <si>
     <t>Competencias</t>
-  </si>
-  <si>
-    <t>Competencias: Comentario de un texto filosófico como fuente.</t>
   </si>
   <si>
     <t xml:space="preserve">Cronología: el fin del Antiguo Régimen </t>
@@ -1844,7 +1789,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1854,17 +1799,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1872,15 +1817,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -1888,15 +1833,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1904,12 +1849,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1928,22 +1873,22 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F20"/>
+      <selection activeCell="D13" sqref="D13:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1963,21 +1908,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="17" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>35</v>
       </c>
       <c r="F2" s="17">
         <v>1</v>
@@ -1989,365 +1934,365 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="17" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="17" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>38</v>
-      </c>
       <c r="E4" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="17" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="17" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="17">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="17" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="17">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="17" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="17">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="17" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="17">
         <v>9</v>
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="E10" s="17" t="s">
         <v>46</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>47</v>
       </c>
       <c r="F10" s="17">
         <v>10</v>
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="17" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="17">
         <v>11</v>
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="17" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="17">
         <v>12</v>
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="17" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="17">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="17" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" s="17">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="17" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" s="17">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="17" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="17">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="17">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="17" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" s="17">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="17" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" s="17">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" s="17">
         <v>21</v>
@@ -2369,16 +2314,16 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A4" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -2389,9 +2334,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>21</v>
@@ -2400,9 +2345,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>21</v>
@@ -2411,7 +2356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
@@ -2422,7 +2367,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
@@ -2455,17 +2400,17 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2476,331 +2421,331 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>34</v>
+      <c r="B2" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="14">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>36</v>
+      <c r="B3" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="14">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>38</v>
+      <c r="B4" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>68</v>
+      <c r="B5" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="14">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>39</v>
+      <c r="B6" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="14">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>40</v>
+      <c r="B7" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>41</v>
+      <c r="B8" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="14">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>42</v>
+      <c r="B9" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="14">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>43</v>
+      <c r="B10" s="17" t="s">
+        <v>42</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="14">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>46</v>
+      <c r="B11" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="14">
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>48</v>
+      <c r="B12" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="14">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>49</v>
+      <c r="B13" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="34"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="14">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>69</v>
+      <c r="B14" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="14">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>52</v>
+      <c r="B15" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="14">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>53</v>
+      <c r="B16" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="14">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>54</v>
+      <c r="B17" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="14">
         <v>17</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>55</v>
+      <c r="B18" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="14">
         <v>18</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>56</v>
+      <c r="B19" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="14">
         <v>19</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>57</v>
+      <c r="B20" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="14">
         <v>20</v>
       </c>
-      <c r="B21" s="14" t="s">
-        <v>58</v>
+      <c r="B21" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="14">
         <v>21</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>59</v>
+      <c r="B22" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="14">
         <v>22</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="14">
         <v>23</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="28"/>
       <c r="B25" s="28"/>
       <c r="C25" s="26"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="25"/>
       <c r="B26" s="25"/>
       <c r="C26" s="26"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="25"/>
       <c r="B27" s="25"/>
       <c r="C27" s="26"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="25"/>
       <c r="B28" s="25"/>
       <c r="C28" s="26"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="25"/>
       <c r="B29" s="25"/>
       <c r="C29" s="26"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="25"/>
       <c r="B30" s="25"/>
       <c r="C30" s="26"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="25"/>
       <c r="B31" s="25"/>
       <c r="C31" s="26"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="25"/>
       <c r="B32" s="25"/>
       <c r="C32" s="26"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="25"/>
       <c r="B33" s="25"/>
       <c r="C33" s="26"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="25"/>
       <c r="B34" s="25"/>
       <c r="C34" s="26"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="25"/>
       <c r="B35" s="25"/>
       <c r="C35" s="26"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="25"/>
       <c r="B36" s="25"/>
       <c r="C36" s="26"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="26"/>
       <c r="B37" s="26"/>
       <c r="C37" s="27"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="26"/>
       <c r="B38" s="26"/>
       <c r="C38" s="27"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="27"/>
@@ -2811,7 +2756,7 @@
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="71" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="71" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -2822,25 +2767,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43:G43"/>
+    <sheetView topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" style="3" customWidth="1"/>
-    <col min="6" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.265625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="42.1328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.86328125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="22" t="s">
         <v>6</v>
       </c>
@@ -2869,12 +2814,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A2" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>24</v>
@@ -2886,12 +2831,12 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A3" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>25</v>
@@ -2903,12 +2848,12 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A4" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>24</v>
@@ -2920,12 +2865,12 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A5" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>27</v>
@@ -2937,16 +2882,16 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C6" s="41"/>
       <c r="D6" s="40" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E6" s="41" t="s">
         <v>24</v>
@@ -2956,16 +2901,16 @@
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A7" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C7" s="41"/>
       <c r="D7" s="40" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E7" s="41" t="s">
         <v>25</v>
@@ -2975,16 +2920,16 @@
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A8" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C8" s="43"/>
       <c r="D8" s="40" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E8" s="44" t="s">
         <v>26</v>
@@ -2992,22 +2937,22 @@
       <c r="F8" s="45"/>
       <c r="G8" s="45"/>
       <c r="H8" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" s="41" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A9" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="40" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E9" s="41" t="s">
         <v>24</v>
@@ -3017,16 +2962,16 @@
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A10" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="40" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E10" s="41" t="s">
         <v>24</v>
@@ -3036,16 +2981,16 @@
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
     </row>
-    <row r="11" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A11" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C11" s="47"/>
       <c r="D11" s="40" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E11" s="44" t="s">
         <v>30</v>
@@ -3055,39 +3000,39 @@
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A12" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C12" s="47"/>
       <c r="D12" s="40" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E12" s="44" t="s">
         <v>29</v>
       </c>
       <c r="F12" s="41"/>
       <c r="G12" s="41"/>
-      <c r="H12" s="46" t="s">
-        <v>73</v>
+      <c r="H12" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A13" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C13" s="47"/>
       <c r="D13" s="40" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E13" s="44" t="s">
         <v>24</v>
@@ -3097,16 +3042,16 @@
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
     </row>
-    <row r="14" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A14" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="40" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E14" s="44" t="s">
         <v>25</v>
@@ -3116,16 +3061,16 @@
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C15" s="47"/>
       <c r="D15" s="40" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E15" s="44" t="s">
         <v>24</v>
@@ -3135,16 +3080,16 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A16" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C16" s="47"/>
       <c r="D16" s="40" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E16" s="44" t="s">
         <v>26</v>
@@ -3152,22 +3097,22 @@
       <c r="F16" s="45"/>
       <c r="G16" s="45"/>
       <c r="H16" s="46" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C17" s="47"/>
       <c r="D17" s="40" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>24</v>
@@ -3177,16 +3122,16 @@
       <c r="H17" s="46"/>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A18" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C18" s="48"/>
       <c r="D18" s="49" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E18" s="48" t="s">
         <v>29</v>
@@ -3194,18 +3139,18 @@
       <c r="F18" s="48"/>
       <c r="G18" s="48"/>
       <c r="H18" s="46" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="I18" s="48" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A19" s="57" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C19" s="59" t="s">
         <v>24</v>
@@ -3217,12 +3162,12 @@
       <c r="H19" s="59"/>
       <c r="I19" s="59"/>
     </row>
-    <row r="20" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A20" s="60" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C20" s="59" t="s">
         <v>25</v>
@@ -3234,12 +3179,12 @@
       <c r="H20" s="59"/>
       <c r="I20" s="59"/>
     </row>
-    <row r="21" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A21" s="62" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C21" s="59" t="s">
         <v>24</v>
@@ -3251,12 +3196,12 @@
       <c r="H21" s="59"/>
       <c r="I21" s="59"/>
     </row>
-    <row r="22" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A22" s="62" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C22" s="59" t="s">
         <v>29</v>
@@ -3266,18 +3211,18 @@
       <c r="F22" s="59"/>
       <c r="G22" s="59"/>
       <c r="H22" s="59" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="I22" s="59" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A23" s="62" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C23" s="59" t="s">
         <v>30</v>
@@ -3289,16 +3234,16 @@
       <c r="H23" s="84"/>
       <c r="I23" s="84"/>
     </row>
-    <row r="24" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A24" s="62" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="58" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C24" s="59"/>
       <c r="D24" s="63" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E24" s="59" t="s">
         <v>24</v>
@@ -3308,16 +3253,16 @@
       <c r="H24" s="84"/>
       <c r="I24" s="84"/>
     </row>
-    <row r="25" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A25" s="62" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C25" s="59"/>
       <c r="D25" s="63" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E25" s="59" t="s">
         <v>29</v>
@@ -3325,18 +3270,18 @@
       <c r="F25" s="59"/>
       <c r="G25" s="59"/>
       <c r="H25" s="59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25" s="59" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A26" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C26" s="32" t="s">
         <v>24</v>
@@ -3348,12 +3293,12 @@
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
     </row>
-    <row r="27" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A27" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C27" s="32" t="s">
         <v>25</v>
@@ -3365,16 +3310,16 @@
       <c r="H27" s="32"/>
       <c r="I27" s="32"/>
     </row>
-    <row r="28" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A28" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C28" s="32"/>
       <c r="D28" s="54" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>24</v>
@@ -3384,16 +3329,16 @@
       <c r="H28" s="32"/>
       <c r="I28" s="32"/>
     </row>
-    <row r="29" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A29" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C29" s="32"/>
       <c r="D29" s="54" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E29" s="32" t="s">
         <v>30</v>
@@ -3403,16 +3348,16 @@
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
     </row>
-    <row r="30" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A30" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C30" s="32"/>
       <c r="D30" s="55" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="E30" s="32" t="s">
         <v>24</v>
@@ -3422,16 +3367,16 @@
       <c r="H30" s="32"/>
       <c r="I30" s="32"/>
     </row>
-    <row r="31" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A31" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="55" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="E31" s="32" t="s">
         <v>25</v>
@@ -3441,16 +3386,16 @@
       <c r="H31" s="32"/>
       <c r="I31" s="32"/>
     </row>
-    <row r="32" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A32" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="55" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="E32" s="32" t="s">
         <v>27</v>
@@ -3460,16 +3405,16 @@
       <c r="H32" s="32"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A33" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="55" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E33" s="32" t="s">
         <v>24</v>
@@ -3479,16 +3424,16 @@
       <c r="H33" s="32"/>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A34" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C34" s="32"/>
       <c r="D34" s="56" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E34" s="85" t="s">
         <v>29</v>
@@ -3496,18 +3441,18 @@
       <c r="F34" s="32"/>
       <c r="G34" s="32"/>
       <c r="H34" s="87" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="I34" s="32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A35" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C35" s="66" t="s">
         <v>24</v>
@@ -3518,13 +3463,14 @@
       <c r="G35" s="66"/>
       <c r="H35" s="66"/>
       <c r="I35" s="66"/>
-    </row>
-    <row r="36" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K35" s="53"/>
+    </row>
+    <row r="36" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A36" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C36" s="66" t="s">
         <v>25</v>
@@ -3535,13 +3481,14 @@
       <c r="G36" s="66"/>
       <c r="H36" s="66"/>
       <c r="I36" s="66"/>
-    </row>
-    <row r="37" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K36" s="53"/>
+    </row>
+    <row r="37" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A37" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B37" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C37" s="66" t="s">
         <v>24</v>
@@ -3552,17 +3499,18 @@
       <c r="G37" s="66"/>
       <c r="H37" s="66"/>
       <c r="I37" s="66"/>
-    </row>
-    <row r="38" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K37" s="53"/>
+    </row>
+    <row r="38" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A38" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B38" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C38" s="66"/>
       <c r="D38" s="69" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E38" s="66" t="s">
         <v>24</v>
@@ -3571,17 +3519,18 @@
       <c r="G38" s="66"/>
       <c r="H38" s="66"/>
       <c r="I38" s="66"/>
-    </row>
-    <row r="39" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K38" s="53"/>
+    </row>
+    <row r="39" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A39" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C39" s="66"/>
       <c r="D39" s="69" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E39" s="66" t="s">
         <v>26</v>
@@ -3589,22 +3538,23 @@
       <c r="F39" s="66"/>
       <c r="G39" s="66"/>
       <c r="H39" s="66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I39" s="66" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K39" s="53"/>
+    </row>
+    <row r="40" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A40" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C40" s="66"/>
       <c r="D40" s="69" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E40" s="66" t="s">
         <v>25</v>
@@ -3613,17 +3563,18 @@
       <c r="G40" s="66"/>
       <c r="H40" s="66"/>
       <c r="I40" s="66"/>
-    </row>
-    <row r="41" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K40" s="53"/>
+    </row>
+    <row r="41" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A41" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B41" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C41" s="66"/>
       <c r="D41" s="69" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E41" s="66" t="s">
         <v>24</v>
@@ -3632,17 +3583,18 @@
       <c r="G41" s="66"/>
       <c r="H41" s="66"/>
       <c r="I41" s="66"/>
-    </row>
-    <row r="42" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K41" s="53"/>
+    </row>
+    <row r="42" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A42" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C42" s="66"/>
       <c r="D42" s="69" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E42" s="66" t="s">
         <v>29</v>
@@ -3650,22 +3602,23 @@
       <c r="F42" s="66"/>
       <c r="G42" s="66"/>
       <c r="H42" s="69" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I42" s="66" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K42" s="53"/>
+    </row>
+    <row r="43" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A43" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C43" s="66"/>
       <c r="D43" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E43" s="66" t="s">
         <v>24</v>
@@ -3674,17 +3627,18 @@
       <c r="G43" s="66"/>
       <c r="H43" s="66"/>
       <c r="I43" s="66"/>
-    </row>
-    <row r="44" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K43" s="53"/>
+    </row>
+    <row r="44" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A44" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C44" s="66"/>
       <c r="D44" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E44" s="66" t="s">
         <v>30</v>
@@ -3693,17 +3647,18 @@
       <c r="G44" s="66"/>
       <c r="H44" s="66"/>
       <c r="I44" s="66"/>
-    </row>
-    <row r="45" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K44" s="53"/>
+    </row>
+    <row r="45" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A45" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B45" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C45" s="66"/>
       <c r="D45" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E45" s="66" t="s">
         <v>26</v>
@@ -3711,22 +3666,23 @@
       <c r="F45" s="66"/>
       <c r="G45" s="66"/>
       <c r="H45" s="66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I45" s="66" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K45" s="53"/>
+    </row>
+    <row r="46" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A46" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C46" s="66"/>
       <c r="D46" s="65" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E46" s="66" t="s">
         <v>24</v>
@@ -3735,17 +3691,18 @@
       <c r="G46" s="66"/>
       <c r="H46" s="66"/>
       <c r="I46" s="66"/>
-    </row>
-    <row r="47" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K46" s="53"/>
+    </row>
+    <row r="47" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A47" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B47" s="65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C47" s="66"/>
       <c r="D47" s="69" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E47" s="66" t="s">
         <v>29</v>
@@ -3753,18 +3710,19 @@
       <c r="F47" s="66"/>
       <c r="G47" s="66"/>
       <c r="H47" s="88" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="I47" s="66" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K47" s="53"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A48" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B48" s="33" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>24</v>
@@ -3775,17 +3733,18 @@
       <c r="G48" s="14"/>
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K48" s="53"/>
+    </row>
+    <row r="49" spans="1:11" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A49" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="38" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>24</v>
@@ -3794,17 +3753,18 @@
       <c r="G49" s="14"/>
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K49" s="53"/>
+    </row>
+    <row r="50" spans="1:11" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A50" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="38" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>29</v>
@@ -3812,18 +3772,19 @@
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
       <c r="H50" s="14" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="I50" s="14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K50" s="53"/>
+    </row>
+    <row r="51" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A51" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B51" s="65" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C51" s="70" t="s">
         <v>24</v>
@@ -3834,17 +3795,18 @@
       <c r="G51" s="70"/>
       <c r="H51" s="70"/>
       <c r="I51" s="70"/>
-    </row>
-    <row r="52" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K51" s="53"/>
+    </row>
+    <row r="52" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A52" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C52" s="70"/>
       <c r="D52" s="71" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E52" s="70" t="s">
         <v>24</v>
@@ -3853,17 +3815,18 @@
       <c r="G52" s="70"/>
       <c r="H52" s="70"/>
       <c r="I52" s="70"/>
-    </row>
-    <row r="53" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K52" s="53"/>
+    </row>
+    <row r="53" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A53" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B53" s="65" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C53" s="70"/>
       <c r="D53" s="71" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E53" s="70" t="s">
         <v>25</v>
@@ -3872,17 +3835,18 @@
       <c r="G53" s="70"/>
       <c r="H53" s="70"/>
       <c r="I53" s="70"/>
-    </row>
-    <row r="54" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K53" s="53"/>
+    </row>
+    <row r="54" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A54" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B54" s="65" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C54" s="70"/>
       <c r="D54" s="71" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E54" s="70" t="s">
         <v>24</v>
@@ -3891,17 +3855,18 @@
       <c r="G54" s="70"/>
       <c r="H54" s="70"/>
       <c r="I54" s="70"/>
-    </row>
-    <row r="55" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K54" s="53"/>
+    </row>
+    <row r="55" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A55" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B55" s="65" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C55" s="70"/>
       <c r="D55" s="71" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E55" s="70" t="s">
         <v>30</v>
@@ -3910,17 +3875,18 @@
       <c r="G55" s="70"/>
       <c r="H55" s="70"/>
       <c r="I55" s="70"/>
-    </row>
-    <row r="56" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K55" s="53"/>
+    </row>
+    <row r="56" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A56" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B56" s="65" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C56" s="70"/>
       <c r="D56" s="71" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E56" s="70" t="s">
         <v>29</v>
@@ -3928,22 +3894,23 @@
       <c r="F56" s="70"/>
       <c r="G56" s="70"/>
       <c r="H56" s="70" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="I56" s="70" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K56" s="53"/>
+    </row>
+    <row r="57" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A57" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B57" s="65" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C57" s="70"/>
       <c r="D57" s="65" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E57" s="70" t="s">
         <v>24</v>
@@ -3952,17 +3919,18 @@
       <c r="G57" s="70"/>
       <c r="H57" s="70"/>
       <c r="I57" s="70"/>
-    </row>
-    <row r="58" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K57" s="53"/>
+    </row>
+    <row r="58" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A58" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B58" s="65" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C58" s="70"/>
       <c r="D58" s="65" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E58" s="70" t="s">
         <v>27</v>
@@ -3971,17 +3939,18 @@
       <c r="G58" s="70"/>
       <c r="H58" s="70"/>
       <c r="I58" s="70"/>
-    </row>
-    <row r="59" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K58" s="53"/>
+    </row>
+    <row r="59" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A59" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B59" s="65" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C59" s="70"/>
       <c r="D59" s="65" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E59" s="70" t="s">
         <v>24</v>
@@ -3990,34 +3959,38 @@
       <c r="G59" s="70"/>
       <c r="H59" s="70"/>
       <c r="I59" s="70"/>
-    </row>
-    <row r="60" spans="1:9" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K59" s="53"/>
+    </row>
+    <row r="60" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A60" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B60" s="65" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C60" s="70"/>
       <c r="D60" s="71" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E60" s="86" t="s">
         <v>29</v>
       </c>
       <c r="F60" s="70"/>
       <c r="G60" s="70"/>
-      <c r="H60" s="70"/>
+      <c r="H60" s="70" t="s">
+        <v>49</v>
+      </c>
       <c r="I60" s="70" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K60" s="53"/>
+    </row>
+    <row r="61" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A61" s="51" t="s">
         <v>31</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>24</v>
@@ -4028,13 +4001,14 @@
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
-    </row>
-    <row r="62" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K61" s="53"/>
+    </row>
+    <row r="62" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="51" t="s">
         <v>31</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>25</v>
@@ -4045,13 +4019,14 @@
       <c r="G62" s="15"/>
       <c r="H62" s="15"/>
       <c r="I62" s="15"/>
-    </row>
-    <row r="63" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K62" s="53"/>
+    </row>
+    <row r="63" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A63" s="51" t="s">
         <v>31</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>24</v>
@@ -4062,13 +4037,14 @@
       <c r="G63" s="15"/>
       <c r="H63" s="15"/>
       <c r="I63" s="15"/>
-    </row>
-    <row r="64" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K63" s="53"/>
+    </row>
+    <row r="64" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A64" s="51" t="s">
         <v>31</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>29</v>
@@ -4078,22 +4054,23 @@
       <c r="F64" s="73"/>
       <c r="G64" s="15"/>
       <c r="H64" s="15" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="I64" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K64" s="53"/>
+    </row>
+    <row r="65" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A65" s="51" t="s">
         <v>31</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="16" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E65" s="72" t="s">
         <v>24</v>
@@ -4102,19 +4079,20 @@
       <c r="G65" s="15"/>
       <c r="H65" s="15"/>
       <c r="I65" s="15"/>
-    </row>
-    <row r="66" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K65" s="53"/>
+    </row>
+    <row r="66" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A66" s="51" t="s">
         <v>31</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E66" s="15" t="s">
         <v>29</v>
@@ -4122,18 +4100,19 @@
       <c r="F66" s="73"/>
       <c r="G66" s="15"/>
       <c r="H66" s="15" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="I66" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K66" s="53"/>
+    </row>
+    <row r="67" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A67" s="74" t="s">
         <v>31</v>
       </c>
       <c r="B67" s="75" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C67" s="76" t="s">
         <v>24</v>
@@ -4144,13 +4123,14 @@
       <c r="G67" s="76"/>
       <c r="H67" s="76"/>
       <c r="I67" s="76"/>
-    </row>
-    <row r="68" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K67" s="53"/>
+    </row>
+    <row r="68" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A68" s="74" t="s">
         <v>31</v>
       </c>
       <c r="B68" s="75" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C68" s="80" t="s">
         <v>25</v>
@@ -4161,13 +4141,14 @@
       <c r="G68" s="81"/>
       <c r="H68" s="81"/>
       <c r="I68" s="81"/>
-    </row>
-    <row r="69" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K68" s="53"/>
+    </row>
+    <row r="69" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A69" s="74" t="s">
         <v>31</v>
       </c>
       <c r="B69" s="75" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C69" s="76" t="s">
         <v>24</v>
@@ -4178,13 +4159,14 @@
       <c r="G69" s="76"/>
       <c r="H69" s="76"/>
       <c r="I69" s="76"/>
-    </row>
-    <row r="70" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K69" s="53"/>
+    </row>
+    <row r="70" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A70" s="74" t="s">
         <v>31</v>
       </c>
       <c r="B70" s="75" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C70" s="76" t="s">
         <v>26</v>
@@ -4194,18 +4176,19 @@
       <c r="F70" s="76"/>
       <c r="G70" s="76"/>
       <c r="H70" s="76" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="I70" s="76" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K70" s="53"/>
+    </row>
+    <row r="71" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A71" s="74" t="s">
         <v>31</v>
       </c>
       <c r="B71" s="75" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C71" s="76" t="s">
         <v>26</v>
@@ -4215,22 +4198,23 @@
       <c r="F71" s="76"/>
       <c r="G71" s="76"/>
       <c r="H71" s="76" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="I71" s="76" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K71" s="53"/>
+    </row>
+    <row r="72" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A72" s="74" t="s">
         <v>31</v>
       </c>
       <c r="B72" s="75" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C72" s="76"/>
       <c r="D72" s="75" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="E72" s="77" t="s">
         <v>24</v>
@@ -4239,17 +4223,18 @@
       <c r="G72" s="76"/>
       <c r="H72" s="76"/>
       <c r="I72" s="76"/>
-    </row>
-    <row r="73" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K72" s="53"/>
+    </row>
+    <row r="73" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A73" s="74" t="s">
         <v>31</v>
       </c>
       <c r="B73" s="75" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C73" s="76"/>
       <c r="D73" s="75" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="E73" s="76" t="s">
         <v>29</v>
@@ -4257,18 +4242,19 @@
       <c r="F73" s="76"/>
       <c r="G73" s="76"/>
       <c r="H73" s="76" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="I73" s="76" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K73" s="53"/>
+    </row>
+    <row r="74" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A74" s="74" t="s">
         <v>31</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>24</v>
@@ -4279,13 +4265,14 @@
       <c r="G74" s="15"/>
       <c r="H74" s="15"/>
       <c r="I74" s="15"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K74" s="53"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>29</v>
@@ -4295,18 +4282,20 @@
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
       <c r="H75" s="15" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="I75" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" s="79"/>
+      <c r="K75" s="53"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>29</v>
@@ -4316,13 +4305,15 @@
       <c r="F76" s="15"/>
       <c r="G76" s="15"/>
       <c r="H76" s="15" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="I76" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76" s="79"/>
+      <c r="K76" s="53"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" s="24" t="s">
         <v>31</v>
       </c>
@@ -4336,14 +4327,12 @@
       <c r="E77" s="16"/>
       <c r="F77" s="16"/>
       <c r="G77" s="16"/>
-      <c r="H77" s="16" t="s">
-        <v>22</v>
-      </c>
+      <c r="H77" s="16"/>
       <c r="I77" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" s="24" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Esqueleto guion 1 Grado 9
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasSociales\fuentes\contenidos\grado08\guion01\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19082" windowHeight="5956" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="5955" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1789,7 +1784,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1800,16 +1795,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1817,7 +1812,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
@@ -1825,7 +1820,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -1833,7 +1828,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -1841,7 +1836,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1849,7 +1844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -1873,22 +1868,22 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:D20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.73046875" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1908,7 +1903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>43</v>
       </c>
@@ -1934,7 +1929,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>43</v>
       </c>
@@ -1954,7 +1949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>43</v>
       </c>
@@ -1974,7 +1969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>43</v>
       </c>
@@ -1994,7 +1989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>43</v>
       </c>
@@ -2014,7 +2009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>43</v>
       </c>
@@ -2034,7 +2029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>43</v>
       </c>
@@ -2054,7 +2049,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>43</v>
       </c>
@@ -2075,7 +2070,7 @@
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>43</v>
       </c>
@@ -2096,7 +2091,7 @@
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>43</v>
       </c>
@@ -2117,7 +2112,7 @@
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>43</v>
       </c>
@@ -2138,7 +2133,7 @@
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>43</v>
       </c>
@@ -2158,7 +2153,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>43</v>
       </c>
@@ -2178,7 +2173,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>43</v>
       </c>
@@ -2198,7 +2193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>43</v>
       </c>
@@ -2218,7 +2213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>43</v>
       </c>
@@ -2238,7 +2233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>43</v>
       </c>
@@ -2258,7 +2253,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>43</v>
       </c>
@@ -2278,7 +2273,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>43</v>
       </c>
@@ -2314,16 +2309,16 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.1328125" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" customWidth="1"/>
+    <col min="1" max="1" width="66.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.95" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -2334,7 +2329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>57</v>
       </c>
@@ -2345,7 +2340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>58</v>
       </c>
@@ -2356,7 +2351,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
@@ -2367,7 +2362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
@@ -2400,17 +2395,17 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.265625" customWidth="1"/>
-    <col min="3" max="3" width="19.265625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="15.95" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2421,7 +2416,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -2432,7 +2427,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -2443,7 +2438,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -2454,7 +2449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.45">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -2465,7 +2460,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -2476,7 +2471,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -2487,7 +2482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -2498,7 +2493,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -2509,7 +2504,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -2520,7 +2515,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -2531,7 +2526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -2542,7 +2537,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -2554,7 +2549,7 @@
       </c>
       <c r="D13" s="34"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.45">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -2565,7 +2560,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>14</v>
       </c>
@@ -2576,7 +2571,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -2587,7 +2582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>16</v>
       </c>
@@ -2598,7 +2593,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -2609,7 +2604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -2620,7 +2615,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -2631,7 +2626,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -2642,7 +2637,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -2653,7 +2648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -2664,7 +2659,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>23</v>
       </c>
@@ -2675,77 +2670,77 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
       <c r="B25" s="28"/>
       <c r="C25" s="26"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="25"/>
       <c r="C26" s="26"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="25"/>
       <c r="C27" s="26"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
       <c r="B28" s="25"/>
       <c r="C28" s="26"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="25"/>
       <c r="C29" s="26"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="25"/>
       <c r="C30" s="26"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="25"/>
       <c r="C31" s="26"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="25"/>
       <c r="C32" s="26"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="25"/>
       <c r="C33" s="26"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="25"/>
       <c r="C34" s="26"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="25"/>
       <c r="C35" s="26"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="25"/>
       <c r="C36" s="26"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="26"/>
       <c r="B37" s="26"/>
       <c r="C37" s="27"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
       <c r="B38" s="26"/>
       <c r="C38" s="27"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="27"/>
@@ -2769,23 +2764,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.265625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="42.1328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33.86328125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="17.86328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.1328125" customWidth="1"/>
-    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" style="3" customWidth="1"/>
+    <col min="6" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="15.95" x14ac:dyDescent="0.5">
       <c r="A1" s="22" t="s">
         <v>6</v>
       </c>
@@ -2814,7 +2809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>31</v>
       </c>
@@ -2831,7 +2826,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>31</v>
       </c>
@@ -2848,7 +2843,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>31</v>
       </c>
@@ -2865,7 +2860,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>31</v>
       </c>
@@ -2882,7 +2877,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>31</v>
       </c>
@@ -2901,7 +2896,7 @@
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>31</v>
       </c>
@@ -2920,7 +2915,7 @@
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>31</v>
       </c>
@@ -2943,7 +2938,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>31</v>
       </c>
@@ -2962,7 +2957,7 @@
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>31</v>
       </c>
@@ -2981,7 +2976,7 @@
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
     </row>
-    <row r="11" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>31</v>
       </c>
@@ -3000,7 +2995,7 @@
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>31</v>
       </c>
@@ -3023,7 +3018,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>31</v>
       </c>
@@ -3042,7 +3037,7 @@
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
     </row>
-    <row r="14" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>31</v>
       </c>
@@ -3061,7 +3056,7 @@
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>31</v>
       </c>
@@ -3080,7 +3075,7 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>31</v>
       </c>
@@ -3103,7 +3098,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>31</v>
       </c>
@@ -3122,7 +3117,7 @@
       <c r="H17" s="46"/>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" s="42" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>31</v>
       </c>
@@ -3145,7 +3140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
         <v>31</v>
       </c>
@@ -3162,7 +3157,7 @@
       <c r="H19" s="59"/>
       <c r="I19" s="59"/>
     </row>
-    <row r="20" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
         <v>31</v>
       </c>
@@ -3179,7 +3174,7 @@
       <c r="H20" s="59"/>
       <c r="I20" s="59"/>
     </row>
-    <row r="21" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="62" t="s">
         <v>31</v>
       </c>
@@ -3196,7 +3191,7 @@
       <c r="H21" s="59"/>
       <c r="I21" s="59"/>
     </row>
-    <row r="22" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="62" t="s">
         <v>31</v>
       </c>
@@ -3217,7 +3212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="62" t="s">
         <v>31</v>
       </c>
@@ -3234,7 +3229,7 @@
       <c r="H23" s="84"/>
       <c r="I23" s="84"/>
     </row>
-    <row r="24" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="62" t="s">
         <v>31</v>
       </c>
@@ -3253,7 +3248,7 @@
       <c r="H24" s="84"/>
       <c r="I24" s="84"/>
     </row>
-    <row r="25" spans="1:9" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="62" t="s">
         <v>31</v>
       </c>
@@ -3276,7 +3271,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="52" t="s">
         <v>31</v>
       </c>
@@ -3293,7 +3288,7 @@
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
     </row>
-    <row r="27" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="52" t="s">
         <v>31</v>
       </c>
@@ -3310,7 +3305,7 @@
       <c r="H27" s="32"/>
       <c r="I27" s="32"/>
     </row>
-    <row r="28" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
         <v>31</v>
       </c>
@@ -3329,7 +3324,7 @@
       <c r="H28" s="32"/>
       <c r="I28" s="32"/>
     </row>
-    <row r="29" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
         <v>31</v>
       </c>
@@ -3348,7 +3343,7 @@
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
     </row>
-    <row r="30" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="52" t="s">
         <v>31</v>
       </c>
@@ -3367,7 +3362,7 @@
       <c r="H30" s="32"/>
       <c r="I30" s="32"/>
     </row>
-    <row r="31" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="52" t="s">
         <v>31</v>
       </c>
@@ -3386,7 +3381,7 @@
       <c r="H31" s="32"/>
       <c r="I31" s="32"/>
     </row>
-    <row r="32" spans="1:9" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
         <v>31</v>
       </c>
@@ -3405,7 +3400,7 @@
       <c r="H32" s="32"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" spans="1:11" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
         <v>31</v>
       </c>
@@ -3424,7 +3419,7 @@
       <c r="H33" s="32"/>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" spans="1:11" s="53" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
         <v>31</v>
       </c>
@@ -3447,7 +3442,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" s="68" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A35" s="64" t="s">
         <v>31</v>
       </c>
@@ -3465,7 +3460,7 @@
       <c r="I35" s="66"/>
       <c r="K35" s="53"/>
     </row>
-    <row r="36" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" s="68" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A36" s="64" t="s">
         <v>31</v>
       </c>
@@ -3483,7 +3478,7 @@
       <c r="I36" s="66"/>
       <c r="K36" s="53"/>
     </row>
-    <row r="37" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" s="68" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A37" s="64" t="s">
         <v>31</v>
       </c>
@@ -3501,7 +3496,7 @@
       <c r="I37" s="66"/>
       <c r="K37" s="53"/>
     </row>
-    <row r="38" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="64" t="s">
         <v>31</v>
       </c>
@@ -3521,7 +3516,7 @@
       <c r="I38" s="66"/>
       <c r="K38" s="53"/>
     </row>
-    <row r="39" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="64" t="s">
         <v>31</v>
       </c>
@@ -3545,7 +3540,7 @@
       </c>
       <c r="K39" s="53"/>
     </row>
-    <row r="40" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="64" t="s">
         <v>31</v>
       </c>
@@ -3565,7 +3560,7 @@
       <c r="I40" s="66"/>
       <c r="K40" s="53"/>
     </row>
-    <row r="41" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="64" t="s">
         <v>31</v>
       </c>
@@ -3585,7 +3580,7 @@
       <c r="I41" s="66"/>
       <c r="K41" s="53"/>
     </row>
-    <row r="42" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="64" t="s">
         <v>31</v>
       </c>
@@ -3609,7 +3604,7 @@
       </c>
       <c r="K42" s="53"/>
     </row>
-    <row r="43" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="64" t="s">
         <v>31</v>
       </c>
@@ -3629,7 +3624,7 @@
       <c r="I43" s="66"/>
       <c r="K43" s="53"/>
     </row>
-    <row r="44" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="64" t="s">
         <v>31</v>
       </c>
@@ -3649,7 +3644,7 @@
       <c r="I44" s="66"/>
       <c r="K44" s="53"/>
     </row>
-    <row r="45" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="64" t="s">
         <v>31</v>
       </c>
@@ -3673,7 +3668,7 @@
       </c>
       <c r="K45" s="53"/>
     </row>
-    <row r="46" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="64" t="s">
         <v>31</v>
       </c>
@@ -3693,7 +3688,7 @@
       <c r="I46" s="66"/>
       <c r="K46" s="53"/>
     </row>
-    <row r="47" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="64" t="s">
         <v>31</v>
       </c>
@@ -3717,7 +3712,7 @@
       </c>
       <c r="K47" s="53"/>
     </row>
-    <row r="48" spans="1:11" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="64" t="s">
         <v>31</v>
       </c>
@@ -3735,7 +3730,7 @@
       <c r="I48" s="14"/>
       <c r="K48" s="53"/>
     </row>
-    <row r="49" spans="1:11" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="64" t="s">
         <v>31</v>
       </c>
@@ -3755,7 +3750,7 @@
       <c r="I49" s="14"/>
       <c r="K49" s="53"/>
     </row>
-    <row r="50" spans="1:11" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="64" t="s">
         <v>31</v>
       </c>
@@ -3779,7 +3774,7 @@
       </c>
       <c r="K50" s="53"/>
     </row>
-    <row r="51" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" s="68" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A51" s="64" t="s">
         <v>31</v>
       </c>
@@ -3797,7 +3792,7 @@
       <c r="I51" s="70"/>
       <c r="K51" s="53"/>
     </row>
-    <row r="52" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" s="68" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A52" s="64" t="s">
         <v>31</v>
       </c>
@@ -3817,7 +3812,7 @@
       <c r="I52" s="70"/>
       <c r="K52" s="53"/>
     </row>
-    <row r="53" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="64" t="s">
         <v>31</v>
       </c>
@@ -3837,7 +3832,7 @@
       <c r="I53" s="70"/>
       <c r="K53" s="53"/>
     </row>
-    <row r="54" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="64" t="s">
         <v>31</v>
       </c>
@@ -3857,7 +3852,7 @@
       <c r="I54" s="70"/>
       <c r="K54" s="53"/>
     </row>
-    <row r="55" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="64" t="s">
         <v>31</v>
       </c>
@@ -3877,7 +3872,7 @@
       <c r="I55" s="70"/>
       <c r="K55" s="53"/>
     </row>
-    <row r="56" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="64" t="s">
         <v>31</v>
       </c>
@@ -3901,7 +3896,7 @@
       </c>
       <c r="K56" s="53"/>
     </row>
-    <row r="57" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="64" t="s">
         <v>31</v>
       </c>
@@ -3921,7 +3916,7 @@
       <c r="I57" s="70"/>
       <c r="K57" s="53"/>
     </row>
-    <row r="58" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="64" t="s">
         <v>31</v>
       </c>
@@ -3941,7 +3936,7 @@
       <c r="I58" s="70"/>
       <c r="K58" s="53"/>
     </row>
-    <row r="59" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="64" t="s">
         <v>31</v>
       </c>
@@ -3961,7 +3956,7 @@
       <c r="I59" s="70"/>
       <c r="K59" s="53"/>
     </row>
-    <row r="60" spans="1:11" s="68" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="64" t="s">
         <v>31</v>
       </c>
@@ -3985,7 +3980,7 @@
       </c>
       <c r="K60" s="53"/>
     </row>
-    <row r="61" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="51" t="s">
         <v>31</v>
       </c>
@@ -4003,7 +3998,7 @@
       <c r="I61" s="15"/>
       <c r="K61" s="53"/>
     </row>
-    <row r="62" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="51" t="s">
         <v>31</v>
       </c>
@@ -4021,7 +4016,7 @@
       <c r="I62" s="15"/>
       <c r="K62" s="53"/>
     </row>
-    <row r="63" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="51" t="s">
         <v>31</v>
       </c>
@@ -4039,7 +4034,7 @@
       <c r="I63" s="15"/>
       <c r="K63" s="53"/>
     </row>
-    <row r="64" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="51" t="s">
         <v>31</v>
       </c>
@@ -4061,7 +4056,7 @@
       </c>
       <c r="K64" s="53"/>
     </row>
-    <row r="65" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="51" t="s">
         <v>31</v>
       </c>
@@ -4081,7 +4076,7 @@
       <c r="I65" s="15"/>
       <c r="K65" s="53"/>
     </row>
-    <row r="66" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="51" t="s">
         <v>31</v>
       </c>
@@ -4107,7 +4102,7 @@
       </c>
       <c r="K66" s="53"/>
     </row>
-    <row r="67" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="74" t="s">
         <v>31</v>
       </c>
@@ -4125,7 +4120,7 @@
       <c r="I67" s="76"/>
       <c r="K67" s="53"/>
     </row>
-    <row r="68" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="74" t="s">
         <v>31</v>
       </c>
@@ -4143,7 +4138,7 @@
       <c r="I68" s="81"/>
       <c r="K68" s="53"/>
     </row>
-    <row r="69" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="74" t="s">
         <v>31</v>
       </c>
@@ -4161,7 +4156,7 @@
       <c r="I69" s="76"/>
       <c r="K69" s="53"/>
     </row>
-    <row r="70" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="74" t="s">
         <v>31</v>
       </c>
@@ -4183,7 +4178,7 @@
       </c>
       <c r="K70" s="53"/>
     </row>
-    <row r="71" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="74" t="s">
         <v>31</v>
       </c>
@@ -4205,7 +4200,7 @@
       </c>
       <c r="K71" s="53"/>
     </row>
-    <row r="72" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="74" t="s">
         <v>31</v>
       </c>
@@ -4225,7 +4220,7 @@
       <c r="I72" s="76"/>
       <c r="K72" s="53"/>
     </row>
-    <row r="73" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="74" t="s">
         <v>31</v>
       </c>
@@ -4249,7 +4244,7 @@
       </c>
       <c r="K73" s="53"/>
     </row>
-    <row r="74" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="74" t="s">
         <v>31</v>
       </c>
@@ -4267,7 +4262,7 @@
       <c r="I74" s="15"/>
       <c r="K74" s="53"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
         <v>31</v>
       </c>
@@ -4290,7 +4285,7 @@
       <c r="J75" s="79"/>
       <c r="K75" s="53"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>31</v>
       </c>
@@ -4313,7 +4308,7 @@
       <c r="J76" s="79"/>
       <c r="K76" s="53"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="24" t="s">
         <v>31</v>
       </c>
@@ -4332,7 +4327,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
CS0801 y CS0802: Actualización de contenidos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/EsqueletoGuion_CS_08_01_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="5955" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="5955" tabRatio="729" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="87">
   <si>
     <t>FICHA</t>
   </si>
@@ -178,12 +178,6 @@
     <t>Refuerza tu aprendizaje: Las revoluciones inglesas</t>
   </si>
   <si>
-    <t>Conoce la revolución americana</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: La revolución americana</t>
-  </si>
-  <si>
     <t>La declaración de los Derechos del Hombre y del Ciudadano</t>
   </si>
   <si>
@@ -259,9 +253,6 @@
     <t>Competencias</t>
   </si>
   <si>
-    <t xml:space="preserve">Cronología: el fin del Antiguo Régimen </t>
-  </si>
-  <si>
     <t>Educación Básica Secundaria</t>
   </si>
   <si>
@@ -284,6 +275,18 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cronología: El fin del Antiguo Régimen </t>
+  </si>
+  <si>
+    <t>Conoce la Revolución americana</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La Revolución americana</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La Revolución francesa</t>
   </si>
 </sst>
 </file>
@@ -1794,7 +1797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1817,7 +1820,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1833,7 +1836,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.45">
@@ -1849,7 +1852,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1867,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,7 +2167,7 @@
         <v>36</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>34</v>
@@ -2184,7 +2187,7 @@
         <v>36</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>34</v>
@@ -2204,7 +2207,7 @@
         <v>36</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>34</v>
@@ -2224,7 +2227,7 @@
         <v>36</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>34</v>
@@ -2244,7 +2247,7 @@
         <v>36</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>34</v>
@@ -2264,7 +2267,7 @@
         <v>36</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>34</v>
@@ -2284,7 +2287,7 @@
         <v>36</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>34</v>
@@ -2331,7 +2334,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>21</v>
@@ -2342,7 +2345,7 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>21</v>
@@ -2395,7 +2398,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,7 +2457,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>21</v>
@@ -2554,7 +2557,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>21</v>
@@ -2576,7 +2579,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>20</v>
@@ -2587,7 +2590,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>20</v>
@@ -2598,7 +2601,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>20</v>
@@ -2609,7 +2612,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>20</v>
@@ -2620,7 +2623,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>20</v>
@@ -2631,7 +2634,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>20</v>
@@ -2642,7 +2645,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>20</v>
@@ -2764,8 +2767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A37" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2814,7 +2817,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>24</v>
@@ -2831,7 +2834,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>25</v>
@@ -2848,7 +2851,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>24</v>
@@ -2865,7 +2868,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>27</v>
@@ -2882,11 +2885,11 @@
         <v>31</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="41"/>
       <c r="D6" s="40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E6" s="41" t="s">
         <v>24</v>
@@ -2901,11 +2904,11 @@
         <v>31</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C7" s="41"/>
       <c r="D7" s="40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E7" s="41" t="s">
         <v>25</v>
@@ -2920,11 +2923,11 @@
         <v>31</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" s="43"/>
       <c r="D8" s="40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E8" s="44" t="s">
         <v>26</v>
@@ -2943,11 +2946,11 @@
         <v>31</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E9" s="41" t="s">
         <v>24</v>
@@ -2962,11 +2965,11 @@
         <v>31</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E10" s="41" t="s">
         <v>24</v>
@@ -2981,11 +2984,11 @@
         <v>31</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C11" s="47"/>
       <c r="D11" s="40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" s="44" t="s">
         <v>30</v>
@@ -3000,11 +3003,11 @@
         <v>31</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C12" s="47"/>
       <c r="D12" s="40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E12" s="44" t="s">
         <v>29</v>
@@ -3023,11 +3026,11 @@
         <v>31</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="47"/>
       <c r="D13" s="40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="44" t="s">
         <v>24</v>
@@ -3042,11 +3045,11 @@
         <v>31</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E14" s="44" t="s">
         <v>25</v>
@@ -3061,11 +3064,11 @@
         <v>31</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C15" s="47"/>
       <c r="D15" s="40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E15" s="44" t="s">
         <v>24</v>
@@ -3080,11 +3083,11 @@
         <v>31</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="47"/>
       <c r="D16" s="40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E16" s="44" t="s">
         <v>26</v>
@@ -3103,11 +3106,11 @@
         <v>31</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C17" s="47"/>
       <c r="D17" s="40" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>24</v>
@@ -3122,11 +3125,11 @@
         <v>31</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C18" s="48"/>
       <c r="D18" s="49" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E18" s="48" t="s">
         <v>29</v>
@@ -3134,7 +3137,7 @@
       <c r="F18" s="48"/>
       <c r="G18" s="48"/>
       <c r="H18" s="46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I18" s="48" t="s">
         <v>21</v>
@@ -3145,7 +3148,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" s="59" t="s">
         <v>24</v>
@@ -3162,7 +3165,7 @@
         <v>31</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20" s="59" t="s">
         <v>25</v>
@@ -3179,7 +3182,7 @@
         <v>31</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C21" s="59" t="s">
         <v>24</v>
@@ -3196,7 +3199,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22" s="59" t="s">
         <v>29</v>
@@ -3206,7 +3209,7 @@
       <c r="F22" s="59"/>
       <c r="G22" s="59"/>
       <c r="H22" s="59" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I22" s="59" t="s">
         <v>20</v>
@@ -3217,7 +3220,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" s="59" t="s">
         <v>30</v>
@@ -3234,11 +3237,11 @@
         <v>31</v>
       </c>
       <c r="B24" s="58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C24" s="59"/>
       <c r="D24" s="63" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E24" s="59" t="s">
         <v>24</v>
@@ -3253,11 +3256,11 @@
         <v>31</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C25" s="59"/>
       <c r="D25" s="63" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E25" s="59" t="s">
         <v>29</v>
@@ -3276,7 +3279,7 @@
         <v>31</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C26" s="32" t="s">
         <v>24</v>
@@ -3293,7 +3296,7 @@
         <v>31</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C27" s="32" t="s">
         <v>25</v>
@@ -3310,11 +3313,11 @@
         <v>31</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C28" s="32"/>
       <c r="D28" s="54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>24</v>
@@ -3329,11 +3332,11 @@
         <v>31</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C29" s="32"/>
       <c r="D29" s="54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E29" s="32" t="s">
         <v>30</v>
@@ -3348,11 +3351,11 @@
         <v>31</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C30" s="32"/>
       <c r="D30" s="55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E30" s="32" t="s">
         <v>24</v>
@@ -3367,11 +3370,11 @@
         <v>31</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E31" s="32" t="s">
         <v>25</v>
@@ -3386,11 +3389,11 @@
         <v>31</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E32" s="32" t="s">
         <v>27</v>
@@ -3405,11 +3408,11 @@
         <v>31</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="55" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E33" s="32" t="s">
         <v>24</v>
@@ -3424,11 +3427,11 @@
         <v>31</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C34" s="32"/>
       <c r="D34" s="56" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E34" s="85" t="s">
         <v>29</v>
@@ -3436,18 +3439,18 @@
       <c r="F34" s="32"/>
       <c r="G34" s="32"/>
       <c r="H34" s="87" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I34" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="65" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="68" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A35" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="65" t="s">
-        <v>69</v>
       </c>
       <c r="C35" s="66" t="s">
         <v>24</v>
@@ -3460,12 +3463,12 @@
       <c r="I35" s="66"/>
       <c r="K35" s="53"/>
     </row>
-    <row r="36" spans="1:11" s="68" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" s="66" t="s">
         <v>25</v>
@@ -3478,12 +3481,12 @@
       <c r="I36" s="66"/>
       <c r="K36" s="53"/>
     </row>
-    <row r="37" spans="1:11" s="68" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B37" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C37" s="66" t="s">
         <v>24</v>
@@ -3501,11 +3504,11 @@
         <v>31</v>
       </c>
       <c r="B38" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C38" s="66"/>
       <c r="D38" s="69" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E38" s="66" t="s">
         <v>24</v>
@@ -3521,11 +3524,11 @@
         <v>31</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C39" s="66"/>
       <c r="D39" s="69" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E39" s="66" t="s">
         <v>26</v>
@@ -3545,11 +3548,11 @@
         <v>31</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C40" s="66"/>
       <c r="D40" s="69" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E40" s="66" t="s">
         <v>25</v>
@@ -3565,11 +3568,11 @@
         <v>31</v>
       </c>
       <c r="B41" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C41" s="66"/>
       <c r="D41" s="69" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E41" s="66" t="s">
         <v>24</v>
@@ -3585,11 +3588,11 @@
         <v>31</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C42" s="66"/>
       <c r="D42" s="69" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E42" s="66" t="s">
         <v>29</v>
@@ -3609,7 +3612,7 @@
         <v>31</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C43" s="66"/>
       <c r="D43" s="65" t="s">
@@ -3629,7 +3632,7 @@
         <v>31</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C44" s="66"/>
       <c r="D44" s="65" t="s">
@@ -3649,7 +3652,7 @@
         <v>31</v>
       </c>
       <c r="B45" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C45" s="66"/>
       <c r="D45" s="65" t="s">
@@ -3673,11 +3676,11 @@
         <v>31</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C46" s="66"/>
       <c r="D46" s="65" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E46" s="66" t="s">
         <v>24</v>
@@ -3693,11 +3696,11 @@
         <v>31</v>
       </c>
       <c r="B47" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C47" s="66"/>
       <c r="D47" s="69" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E47" s="66" t="s">
         <v>29</v>
@@ -3717,7 +3720,7 @@
         <v>31</v>
       </c>
       <c r="B48" s="33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>24</v>
@@ -3735,11 +3738,11 @@
         <v>31</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="38" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>24</v>
@@ -3755,11 +3758,11 @@
         <v>31</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="38" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>29</v>
@@ -3774,12 +3777,12 @@
       </c>
       <c r="K50" s="53"/>
     </row>
-    <row r="51" spans="1:11" s="68" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B51" s="65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C51" s="70" t="s">
         <v>24</v>
@@ -3792,16 +3795,16 @@
       <c r="I51" s="70"/>
       <c r="K51" s="53"/>
     </row>
-    <row r="52" spans="1:11" s="68" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C52" s="70"/>
       <c r="D52" s="71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E52" s="70" t="s">
         <v>24</v>
@@ -3817,11 +3820,11 @@
         <v>31</v>
       </c>
       <c r="B53" s="65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C53" s="70"/>
       <c r="D53" s="71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E53" s="70" t="s">
         <v>25</v>
@@ -3837,11 +3840,11 @@
         <v>31</v>
       </c>
       <c r="B54" s="65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C54" s="70"/>
       <c r="D54" s="71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E54" s="70" t="s">
         <v>24</v>
@@ -3857,11 +3860,11 @@
         <v>31</v>
       </c>
       <c r="B55" s="65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C55" s="70"/>
       <c r="D55" s="71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E55" s="70" t="s">
         <v>30</v>
@@ -3877,11 +3880,11 @@
         <v>31</v>
       </c>
       <c r="B56" s="65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C56" s="70"/>
       <c r="D56" s="71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E56" s="70" t="s">
         <v>29</v>
@@ -3889,7 +3892,7 @@
       <c r="F56" s="70"/>
       <c r="G56" s="70"/>
       <c r="H56" s="70" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I56" s="70" t="s">
         <v>21</v>
@@ -3901,11 +3904,11 @@
         <v>31</v>
       </c>
       <c r="B57" s="65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C57" s="70"/>
       <c r="D57" s="65" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E57" s="70" t="s">
         <v>24</v>
@@ -3921,11 +3924,11 @@
         <v>31</v>
       </c>
       <c r="B58" s="65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C58" s="70"/>
       <c r="D58" s="65" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E58" s="70" t="s">
         <v>27</v>
@@ -3941,11 +3944,11 @@
         <v>31</v>
       </c>
       <c r="B59" s="65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C59" s="70"/>
       <c r="D59" s="65" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E59" s="70" t="s">
         <v>24</v>
@@ -3961,11 +3964,11 @@
         <v>31</v>
       </c>
       <c r="B60" s="65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C60" s="70"/>
       <c r="D60" s="71" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E60" s="86" t="s">
         <v>29</v>
@@ -3985,7 +3988,7 @@
         <v>31</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>24</v>
@@ -4003,7 +4006,7 @@
         <v>31</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>25</v>
@@ -4021,7 +4024,7 @@
         <v>31</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>24</v>
@@ -4039,7 +4042,7 @@
         <v>31</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>29</v>
@@ -4049,7 +4052,7 @@
       <c r="F64" s="73"/>
       <c r="G64" s="15"/>
       <c r="H64" s="15" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="I64" s="15" t="s">
         <v>20</v>
@@ -4061,11 +4064,11 @@
         <v>31</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E65" s="72" t="s">
         <v>24</v>
@@ -4081,13 +4084,13 @@
         <v>31</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E66" s="15" t="s">
         <v>29</v>
@@ -4095,7 +4098,7 @@
       <c r="F66" s="73"/>
       <c r="G66" s="15"/>
       <c r="H66" s="15" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="I66" s="15" t="s">
         <v>20</v>
@@ -4107,7 +4110,7 @@
         <v>31</v>
       </c>
       <c r="B67" s="75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C67" s="76" t="s">
         <v>24</v>
@@ -4125,7 +4128,7 @@
         <v>31</v>
       </c>
       <c r="B68" s="75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C68" s="80" t="s">
         <v>25</v>
@@ -4143,7 +4146,7 @@
         <v>31</v>
       </c>
       <c r="B69" s="75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C69" s="76" t="s">
         <v>24</v>
@@ -4161,7 +4164,7 @@
         <v>31</v>
       </c>
       <c r="B70" s="75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C70" s="76" t="s">
         <v>26</v>
@@ -4171,7 +4174,7 @@
       <c r="F70" s="76"/>
       <c r="G70" s="76"/>
       <c r="H70" s="76" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I70" s="76" t="s">
         <v>20</v>
@@ -4183,7 +4186,7 @@
         <v>31</v>
       </c>
       <c r="B71" s="75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C71" s="76" t="s">
         <v>26</v>
@@ -4193,7 +4196,7 @@
       <c r="F71" s="76"/>
       <c r="G71" s="76"/>
       <c r="H71" s="76" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I71" s="76" t="s">
         <v>20</v>
@@ -4205,11 +4208,11 @@
         <v>31</v>
       </c>
       <c r="B72" s="75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C72" s="76"/>
       <c r="D72" s="75" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E72" s="77" t="s">
         <v>24</v>
@@ -4225,11 +4228,11 @@
         <v>31</v>
       </c>
       <c r="B73" s="75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C73" s="76"/>
       <c r="D73" s="75" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E73" s="76" t="s">
         <v>29</v>
@@ -4237,7 +4240,7 @@
       <c r="F73" s="76"/>
       <c r="G73" s="76"/>
       <c r="H73" s="76" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I73" s="76" t="s">
         <v>20</v>
@@ -4249,7 +4252,7 @@
         <v>31</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>24</v>
@@ -4267,7 +4270,7 @@
         <v>31</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>29</v>
@@ -4277,7 +4280,7 @@
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
       <c r="H75" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I75" s="15" t="s">
         <v>20</v>
@@ -4290,7 +4293,7 @@
         <v>31</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>29</v>
@@ -4300,7 +4303,7 @@
       <c r="F76" s="15"/>
       <c r="G76" s="15"/>
       <c r="H76" s="15" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I76" s="15" t="s">
         <v>20</v>

</xml_diff>